<commit_message>
Add Update Date Button - Fully Functioning
</commit_message>
<xml_diff>
--- a/4-08-2020 (2).xlsx
+++ b/4-08-2020 (2).xlsx
@@ -227,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,12 +237,6 @@
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -256,15 +250,6 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -274,40 +259,13 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -322,25 +280,7 @@
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -358,10 +298,28 @@
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -764,487 +722,484 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="K2" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="4.42578125"/>
-    <col customWidth="1" max="2" min="2" style="11" width="18.5703125"/>
-    <col customWidth="1" max="3" min="3" style="11" width="15.7109375"/>
-    <col customWidth="1" max="4" min="4" style="11" width="9.140625"/>
-    <col customWidth="1" max="5" min="5" style="11" width="15.7109375"/>
-    <col customWidth="1" max="6" min="6" style="11" width="12.140625"/>
-    <col customWidth="1" max="9" min="7" style="11" width="14.140625"/>
-    <col customWidth="1" max="10" min="10" style="11" width="8.140625"/>
-    <col customWidth="1" max="11" min="11" style="11" width="18.140625"/>
-    <col customWidth="1" max="12" min="12" style="11" width="14.140625"/>
-    <col customWidth="1" max="13" min="13" style="11" width="10.85546875"/>
-    <col customWidth="1" max="16384" min="14" style="11" width="9.140625"/>
+    <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
+    <col customWidth="1" max="2" min="2" style="29" width="18.5703125"/>
+    <col customWidth="1" max="3" min="3" style="29" width="15.7109375"/>
+    <col customWidth="1" max="4" min="4" style="29" width="9.140625"/>
+    <col customWidth="1" max="5" min="5" style="29" width="15.7109375"/>
+    <col customWidth="1" max="6" min="6" style="29" width="12.140625"/>
+    <col customWidth="1" max="9" min="7" style="29" width="14.140625"/>
+    <col customWidth="1" max="10" min="10" style="29" width="8.140625"/>
+    <col customWidth="1" max="11" min="11" style="29" width="18.140625"/>
+    <col customWidth="1" max="12" min="12" style="29" width="14.140625"/>
+    <col customWidth="1" max="13" min="13" style="29" width="10.85546875"/>
+    <col customWidth="1" max="14" min="14" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="28" t="inlineStr">
         <is>
           <t>GREATER HYDERABAD MUNICIPAL CORPORATION</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="30.75" r="2">
-      <c r="B2" s="31" t="inlineStr">
+      <c r="B2" s="26" t="inlineStr">
         <is>
           <t>Name of the Zone:Charminar Zone</t>
         </is>
       </c>
-      <c r="C2" s="44" t="n"/>
-      <c r="J2" s="6" t="inlineStr">
+      <c r="C2" s="27" t="n"/>
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Circle:6</t>
         </is>
       </c>
-      <c r="K2" s="31" t="inlineStr">
-        <is>
-          <t>Date : 2020-09-05</t>
-        </is>
-      </c>
-      <c r="L2" s="44" t="n"/>
+      <c r="K2" s="26" t="inlineStr">
+        <is>
+          <t>09-09-2020</t>
+        </is>
+      </c>
+      <c r="L2" s="27" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="inlineStr">
+      <c r="A3" s="30" t="inlineStr">
         <is>
           <t>SL No</t>
         </is>
       </c>
-      <c r="B3" s="33" t="inlineStr">
+      <c r="B3" s="30" t="inlineStr">
         <is>
           <t>Division Name</t>
         </is>
       </c>
-      <c r="C3" s="33" t="inlineStr">
+      <c r="C3" s="30" t="inlineStr">
         <is>
           <t>PFM-1</t>
         </is>
       </c>
-      <c r="D3" s="45" t="n"/>
-      <c r="E3" s="46" t="n"/>
-      <c r="F3" s="33" t="inlineStr">
+      <c r="D3" s="32" t="n"/>
+      <c r="E3" s="25" t="n"/>
+      <c r="F3" s="30" t="inlineStr">
         <is>
           <t>PFM-2</t>
         </is>
       </c>
-      <c r="G3" s="45" t="n"/>
-      <c r="H3" s="46" t="n"/>
-      <c r="I3" s="33" t="inlineStr">
+      <c r="G3" s="32" t="n"/>
+      <c r="H3" s="25" t="n"/>
+      <c r="I3" s="30" t="inlineStr">
         <is>
           <t>VMF</t>
         </is>
       </c>
-      <c r="J3" s="45" t="n"/>
-      <c r="K3" s="46" t="n"/>
-      <c r="L3" s="33" t="n"/>
+      <c r="J3" s="32" t="n"/>
+      <c r="K3" s="25" t="n"/>
+      <c r="L3" s="30" t="n"/>
     </row>
     <row customHeight="1" ht="45" r="4">
-      <c r="A4" s="47" t="n"/>
-      <c r="B4" s="47" t="n"/>
-      <c r="C4" s="33" t="inlineStr">
+      <c r="A4" s="31" t="n"/>
+      <c r="B4" s="31" t="n"/>
+      <c r="C4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="D4" s="33" t="inlineStr">
+      <c r="D4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="E4" s="33" t="inlineStr">
+      <c r="E4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="F4" s="33" t="inlineStr">
+      <c r="F4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="G4" s="33" t="inlineStr">
+      <c r="G4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="H4" s="33" t="inlineStr">
+      <c r="H4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
+      <c r="I4" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">TL Name &amp; Mobile </t>
         </is>
       </c>
-      <c r="J4" s="33" t="inlineStr">
+      <c r="J4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="K4" s="33" t="inlineStr">
+      <c r="K4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="L4" s="33" t="inlineStr">
+      <c r="L4" s="30" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="135.75" r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="inlineStr">
+      <c r="B5" s="9" t="inlineStr">
         <is>
           <t>Saidabad-24</t>
         </is>
       </c>
-      <c r="C5" s="21" t="inlineStr">
+      <c r="C5" s="13" t="inlineStr">
         <is>
           <t>Kaldev &amp;  
 9666977784</t>
         </is>
       </c>
-      <c r="D5" s="21" t="n">
+      <c r="D5" s="13" t="n">
         <v>2.4</v>
       </c>
-      <c r="E5" s="1" t="inlineStr">
+      <c r="E5" s="33" t="inlineStr">
         <is>
           <t>Bholaxmi nagar</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="33" t="inlineStr">
         <is>
           <t>Kanna 
 8555050335</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="33" t="n">
         <v>2.3</v>
       </c>
-      <c r="H5" s="1" t="inlineStr">
+      <c r="H5" s="33" t="inlineStr">
         <is>
           <t>Asmanggt</t>
         </is>
       </c>
-      <c r="I5" s="1" t="n"/>
-      <c r="J5" s="1" t="n"/>
-      <c r="K5" s="1" t="n"/>
-      <c r="L5" s="1" t="n"/>
+      <c r="I5" s="33" t="n"/>
+      <c r="J5" s="33" t="n"/>
+      <c r="K5" s="33" t="n"/>
+      <c r="L5" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="113.25" r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="14" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>Moosamrambagh-25</t>
         </is>
       </c>
-      <c r="C6" s="21" t="inlineStr">
+      <c r="C6" s="13" t="inlineStr">
         <is>
           <t>Jagadish &amp; 
 9505860994</t>
         </is>
       </c>
-      <c r="D6" s="21" t="n">
+      <c r="D6" s="13" t="n">
         <v>2.3</v>
       </c>
-      <c r="E6" s="21" t="inlineStr">
+      <c r="E6" s="13" t="inlineStr">
         <is>
           <t>Sbi colony</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="33" t="inlineStr">
         <is>
           <t>BalrajuNimmarajula
 9912400458</t>
         </is>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H6" s="1" t="inlineStr">
+      <c r="H6" s="33" t="inlineStr">
         <is>
           <t>Sai nagar</t>
         </is>
       </c>
-      <c r="I6" s="1" t="inlineStr">
+      <c r="I6" s="33" t="inlineStr">
         <is>
           <t>Zubbair</t>
         </is>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="J6" s="33" t="n">
         <v>16.2</v>
       </c>
-      <c r="K6" s="14" t="inlineStr">
+      <c r="K6" s="9" t="inlineStr">
         <is>
           <t>Shalivana nagar,Moosarnbagh,Dilsuknagar,Gandhi nagar</t>
         </is>
       </c>
-      <c r="L6" s="1" t="n"/>
+      <c r="L6" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="151.5" r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="inlineStr">
+      <c r="B7" s="9" t="inlineStr">
         <is>
           <t>Old Malakpet-26</t>
         </is>
       </c>
-      <c r="C7" s="21" t="inlineStr">
+      <c r="C7" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">Venugopal &amp; 
 9381278922 </t>
         </is>
       </c>
-      <c r="D7" s="21" t="n">
+      <c r="D7" s="13" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="1" t="inlineStr">
+      <c r="E7" s="33" t="inlineStr">
         <is>
           <t>Zehra nagar</t>
         </is>
       </c>
-      <c r="F7" s="1" t="inlineStr">
+      <c r="F7" s="33" t="inlineStr">
         <is>
           <t>Pratap Pradeep
 9618014392</t>
         </is>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H7" s="1" t="inlineStr">
+      <c r="H7" s="33" t="inlineStr">
         <is>
           <t>Baba nagar</t>
         </is>
       </c>
-      <c r="I7" s="1" t="n"/>
-      <c r="J7" s="1" t="n"/>
-      <c r="K7" s="14" t="n"/>
-      <c r="L7" s="1" t="n"/>
+      <c r="I7" s="33" t="n"/>
+      <c r="J7" s="33" t="n"/>
+      <c r="K7" s="9" t="n"/>
+      <c r="L7" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="14" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>Azampura-28</t>
         </is>
       </c>
-      <c r="C8" s="21" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t>Ganesh &amp; 
 9700484931</t>
         </is>
       </c>
-      <c r="D8" s="21" t="n">
+      <c r="D8" s="13" t="n">
         <v>2.6</v>
       </c>
-      <c r="E8" s="1" t="inlineStr">
+      <c r="E8" s="33" t="inlineStr">
         <is>
           <t>Chanchalguda</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr">
+      <c r="F8" s="33" t="inlineStr">
         <is>
           <t>Srinivas 
 9966481755</t>
         </is>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="33" t="n">
         <v>2.7</v>
       </c>
-      <c r="H8" s="1" t="inlineStr">
+      <c r="H8" s="33" t="inlineStr">
         <is>
           <t>jatpatnagar</t>
         </is>
       </c>
-      <c r="I8" s="1" t="n"/>
-      <c r="J8" s="1" t="n"/>
-      <c r="K8" s="1" t="n"/>
-      <c r="L8" s="1" t="n"/>
+      <c r="I8" s="33" t="n"/>
+      <c r="J8" s="33" t="n"/>
+      <c r="K8" s="33" t="n"/>
+      <c r="L8" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="103.5" r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="14" t="inlineStr">
+      <c r="B9" s="9" t="inlineStr">
         <is>
           <t>Dabeerpura-30</t>
         </is>
       </c>
-      <c r="C9" s="21" t="inlineStr">
+      <c r="C9" s="13" t="inlineStr">
         <is>
           <t>Ramesh &amp; 
 9247821824</t>
         </is>
       </c>
-      <c r="D9" s="21" t="n">
+      <c r="D9" s="13" t="n">
         <v>2.4</v>
       </c>
-      <c r="E9" s="1" t="inlineStr">
+      <c r="E9" s="33" t="inlineStr">
         <is>
           <t>Shanker nagar</t>
         </is>
       </c>
-      <c r="F9" s="1" t="inlineStr">
+      <c r="F9" s="33" t="inlineStr">
         <is>
           <t>Mallesh 
 8019143414</t>
         </is>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H9" s="1" t="inlineStr">
+      <c r="H9" s="33" t="inlineStr">
         <is>
           <t>Shanker nagar new</t>
         </is>
       </c>
-      <c r="I9" s="18" t="inlineStr">
+      <c r="I9" s="11" t="inlineStr">
         <is>
           <t>B.Ravi
 9603268443</t>
         </is>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="J9" s="33" t="n">
         <v>18</v>
       </c>
-      <c r="K9" s="1" t="inlineStr">
+      <c r="K9" s="33" t="inlineStr">
         <is>
           <t>Hussain nagar.Jaber Hotel Daberpura.Darushfa,Zara Nagar,Bada Bazar</t>
         </is>
       </c>
-      <c r="L9" s="1" t="n"/>
+      <c r="L9" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="160.5" r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="14" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>Akberbagh-27</t>
         </is>
       </c>
-      <c r="C10" s="21" t="inlineStr">
+      <c r="C10" s="13" t="inlineStr">
         <is>
           <t>Suresh &amp; 
 9985376352</t>
         </is>
       </c>
-      <c r="D10" s="21" t="n">
+      <c r="D10" s="13" t="n">
         <v>2.2</v>
       </c>
-      <c r="E10" s="1" t="inlineStr">
+      <c r="E10" s="33" t="inlineStr">
         <is>
           <t>Arman tower</t>
         </is>
       </c>
-      <c r="F10" s="1" t="inlineStr">
+      <c r="F10" s="33" t="inlineStr">
         <is>
           <t>Amar 
 6281569970</t>
         </is>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H10" s="1" t="inlineStr">
+      <c r="H10" s="33" t="inlineStr">
         <is>
           <t>Sbi colony</t>
         </is>
       </c>
-      <c r="I10" s="1" t="n"/>
-      <c r="J10" s="1" t="n"/>
-      <c r="K10" s="1" t="n"/>
-      <c r="L10" s="1" t="n"/>
+      <c r="I10" s="33" t="n"/>
+      <c r="J10" s="33" t="n"/>
+      <c r="K10" s="33" t="n"/>
+      <c r="L10" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="93.75" r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="33" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="14" t="inlineStr">
+      <c r="B11" s="9" t="inlineStr">
         <is>
           <t>Chowni-29</t>
         </is>
       </c>
-      <c r="C11" s="21" t="inlineStr">
+      <c r="C11" s="13" t="inlineStr">
         <is>
           <t>Jagadish &amp; 
 8886924293</t>
         </is>
       </c>
-      <c r="D11" s="21" t="n">
+      <c r="D11" s="13" t="n">
         <v>2.7</v>
       </c>
-      <c r="E11" s="1" t="inlineStr">
+      <c r="E11" s="33" t="inlineStr">
         <is>
           <t>Baghe e Jahara</t>
         </is>
       </c>
-      <c r="F11" s="1" t="inlineStr">
+      <c r="F11" s="33" t="inlineStr">
         <is>
           <t>Gopi
 8886923293</t>
         </is>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="33" t="n">
         <v>2.8</v>
       </c>
-      <c r="H11" s="1" t="inlineStr">
+      <c r="H11" s="33" t="inlineStr">
         <is>
           <t>Chowni</t>
         </is>
       </c>
-      <c r="I11" s="1" t="n"/>
-      <c r="J11" s="1" t="n"/>
-      <c r="K11" s="1" t="n"/>
-      <c r="L11" s="1" t="n"/>
+      <c r="I11" s="33" t="n"/>
+      <c r="J11" s="33" t="n"/>
+      <c r="K11" s="33" t="n"/>
+      <c r="L11" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="34.5" r="12">
-      <c r="A12" s="1" t="n"/>
-      <c r="B12" s="30" t="inlineStr">
+      <c r="A12" s="33" t="n"/>
+      <c r="B12" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C12" s="46" t="n"/>
-      <c r="D12" s="30">
+      <c r="C12" s="25" t="n"/>
+      <c r="D12" s="24">
         <f>SUM(D5:D11)</f>
         <v/>
       </c>
-      <c r="E12" s="1" t="n"/>
-      <c r="F12" s="1" t="n"/>
-      <c r="G12" s="33">
+      <c r="E12" s="33" t="n"/>
+      <c r="F12" s="33" t="n"/>
+      <c r="G12" s="30">
         <f>SUM(G5:G11)</f>
         <v/>
       </c>
-      <c r="H12" s="1" t="n"/>
-      <c r="I12" s="1" t="n"/>
-      <c r="J12" s="33">
+      <c r="H12" s="33" t="n"/>
+      <c r="I12" s="33" t="n"/>
+      <c r="J12" s="30">
         <f>SUM(J6:J10)</f>
         <v/>
       </c>
-      <c r="K12" s="1" t="n"/>
-      <c r="L12" s="1" t="n"/>
-    </row>
-    <row r="27">
-      <c r="L27" s="11" t="n"/>
-      <c r="M27" s="11" t="n"/>
+      <c r="K12" s="33" t="n"/>
+      <c r="L12" s="33" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1275,144 +1230,145 @@
       <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="4.42578125"/>
-    <col customWidth="1" max="2" min="2" style="11" width="18.7109375"/>
-    <col customWidth="1" max="3" min="3" style="11" width="15.7109375"/>
-    <col customWidth="1" max="4" min="4" style="11" width="9.140625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="11" width="21.140625"/>
-    <col customWidth="1" max="8" min="6" style="11" width="11.7109375"/>
-    <col customWidth="1" max="10" min="9" style="11" width="14.140625"/>
-    <col customWidth="1" max="11" min="11" style="11" width="18.28515625"/>
-    <col customWidth="1" max="12" min="12" style="11" width="10.7109375"/>
-    <col customWidth="1" max="16384" min="13" style="11" width="9.140625"/>
+    <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
+    <col customWidth="1" max="2" min="2" style="29" width="18.7109375"/>
+    <col customWidth="1" max="3" min="3" style="29" width="15.7109375"/>
+    <col customWidth="1" max="4" min="4" style="29" width="9.140625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="29" width="21.140625"/>
+    <col customWidth="1" max="8" min="6" style="29" width="11.7109375"/>
+    <col customWidth="1" max="10" min="9" style="29" width="14.140625"/>
+    <col customWidth="1" max="11" min="11" style="29" width="18.28515625"/>
+    <col customWidth="1" max="12" min="12" style="29" width="10.7109375"/>
+    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="28" t="inlineStr">
         <is>
           <t>GREATER HYDERABAD MUNICIPAL CORPORATION</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="B2" s="31" t="inlineStr">
+      <c r="B2" s="26" t="inlineStr">
         <is>
           <t>Name of the Zone:Charminar Zone</t>
         </is>
       </c>
-      <c r="C2" s="44" t="n"/>
-      <c r="J2" s="6" t="inlineStr">
+      <c r="C2" s="27" t="n"/>
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Circle:7</t>
         </is>
       </c>
-      <c r="K2" s="31" t="inlineStr">
+      <c r="K2" s="26" t="inlineStr">
         <is>
           <t>Date:4.08.2020</t>
         </is>
       </c>
-      <c r="L2" s="44" t="n"/>
+      <c r="L2" s="27" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="inlineStr">
+      <c r="A3" s="30" t="inlineStr">
         <is>
           <t>SL No</t>
         </is>
       </c>
-      <c r="B3" s="33" t="inlineStr">
+      <c r="B3" s="30" t="inlineStr">
         <is>
           <t>Division Name</t>
         </is>
       </c>
-      <c r="C3" s="33" t="inlineStr">
+      <c r="C3" s="30" t="inlineStr">
         <is>
           <t>PFM-1</t>
         </is>
       </c>
-      <c r="D3" s="45" t="n"/>
-      <c r="E3" s="46" t="n"/>
-      <c r="F3" s="33" t="inlineStr">
+      <c r="D3" s="32" t="n"/>
+      <c r="E3" s="25" t="n"/>
+      <c r="F3" s="30" t="inlineStr">
         <is>
           <t>PFM-2</t>
         </is>
       </c>
-      <c r="G3" s="45" t="n"/>
-      <c r="H3" s="46" t="n"/>
-      <c r="I3" s="33" t="inlineStr">
+      <c r="G3" s="32" t="n"/>
+      <c r="H3" s="25" t="n"/>
+      <c r="I3" s="30" t="inlineStr">
         <is>
           <t>VMF</t>
         </is>
       </c>
-      <c r="J3" s="45" t="n"/>
-      <c r="K3" s="46" t="n"/>
-      <c r="L3" s="33" t="n"/>
+      <c r="J3" s="32" t="n"/>
+      <c r="K3" s="25" t="n"/>
+      <c r="L3" s="30" t="n"/>
     </row>
     <row customHeight="1" ht="29.25" r="4">
-      <c r="A4" s="47" t="n"/>
-      <c r="B4" s="47" t="n"/>
-      <c r="C4" s="33" t="inlineStr">
+      <c r="A4" s="31" t="n"/>
+      <c r="B4" s="31" t="n"/>
+      <c r="C4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="D4" s="33" t="inlineStr">
+      <c r="D4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="E4" s="33" t="inlineStr">
+      <c r="E4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="F4" s="33" t="inlineStr">
+      <c r="F4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="G4" s="33" t="inlineStr">
+      <c r="G4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="H4" s="33" t="inlineStr">
+      <c r="H4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
+      <c r="I4" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">TL Name &amp; Mobile </t>
         </is>
       </c>
-      <c r="J4" s="33" t="inlineStr">
+      <c r="J4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="K4" s="33" t="inlineStr">
+      <c r="K4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="L4" s="33" t="inlineStr">
+      <c r="L4" s="30" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="30" r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="inlineStr">
+      <c r="B5" s="9" t="inlineStr">
         <is>
           <t>Gowlipura-35</t>
         </is>
       </c>
-      <c r="C5" s="21" t="inlineStr">
+      <c r="C5" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">Santosh &amp; 8555856896 </t>
         </is>
@@ -1420,52 +1376,52 @@
       <c r="D5" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E5" s="21" t="inlineStr">
+      <c r="E5" s="13" t="inlineStr">
         <is>
           <t>Kumarwadi Colony</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="33" t="inlineStr">
         <is>
           <t>Prabhakar
 8074162170</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H5" s="1" t="inlineStr">
+      <c r="H5" s="33" t="inlineStr">
         <is>
           <t>Patel Nagar</t>
         </is>
       </c>
-      <c r="I5" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K5" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="n"/>
+      <c r="I5" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J5" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K5" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="39.75" r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="14" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>Rein Bazar-31</t>
         </is>
       </c>
-      <c r="C6" s="21" t="inlineStr">
+      <c r="C6" s="13" t="inlineStr">
         <is>
           <t>Narsimha &amp;  9985089596</t>
         </is>
@@ -1473,52 +1429,52 @@
       <c r="D6" s="3" t="n">
         <v>2.6</v>
       </c>
-      <c r="E6" s="21" t="inlineStr">
+      <c r="E6" s="13" t="inlineStr">
         <is>
           <t>Surya Junghki dhawadi</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="33" t="inlineStr">
         <is>
           <t>Jangiri
 9182142133</t>
         </is>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="33" t="n">
         <v>2.3</v>
       </c>
-      <c r="H6" s="1" t="inlineStr">
+      <c r="H6" s="33" t="inlineStr">
         <is>
           <t>Chandra Chota Nagar</t>
         </is>
       </c>
-      <c r="I6" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K6" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L6" s="48" t="n"/>
+      <c r="I6" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J6" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" s="34" t="n"/>
     </row>
     <row customHeight="1" ht="106.5" r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="inlineStr">
+      <c r="B7" s="9" t="inlineStr">
         <is>
           <t>IS Sadan-38</t>
         </is>
       </c>
-      <c r="C7" s="21" t="inlineStr">
+      <c r="C7" s="13" t="inlineStr">
         <is>
           <t>Shanker
 9701554484</t>
@@ -1527,50 +1483,50 @@
       <c r="D7" s="3" t="n">
         <v>2.2</v>
       </c>
-      <c r="E7" s="21" t="inlineStr">
+      <c r="E7" s="13" t="inlineStr">
         <is>
           <t>Laxmi Nagar</t>
         </is>
       </c>
-      <c r="F7" s="1" t="inlineStr">
+      <c r="F7" s="33" t="inlineStr">
         <is>
           <t>Anjaiah
 9848790134</t>
         </is>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H7" s="21" t="inlineStr">
+      <c r="H7" s="13" t="inlineStr">
         <is>
           <t>Sigareni Colony Huts</t>
         </is>
       </c>
-      <c r="I7" s="15" t="inlineStr">
+      <c r="I7" s="10" t="inlineStr">
         <is>
           <t>Abdul khaja hussain 9160969450</t>
         </is>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="J7" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="1" t="inlineStr">
+      <c r="K7" s="33" t="inlineStr">
         <is>
           <t>VMF fogging not done Due to Machine repaire</t>
         </is>
       </c>
-      <c r="L7" s="48" t="n"/>
+      <c r="L7" s="34" t="n"/>
     </row>
     <row customHeight="1" ht="62.25" r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="14" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>Kurmagdua-37</t>
         </is>
       </c>
-      <c r="C8" s="21" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t>Babu &amp; 7981051446</t>
         </is>
@@ -1583,41 +1539,41 @@
           <t>Medipur Madaanapet</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr">
+      <c r="F8" s="33" t="inlineStr">
         <is>
           <t>Ghouse
 7780195466</t>
         </is>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H8" s="1" t="inlineStr">
+      <c r="H8" s="33" t="inlineStr">
         <is>
           <t>Madannapet Mandi</t>
         </is>
       </c>
-      <c r="I8" s="1" t="inlineStr">
+      <c r="I8" s="33" t="inlineStr">
         <is>
           <t>Purshotham 7013360671</t>
         </is>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="J8" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="K8" s="14" t="n"/>
-      <c r="L8" s="48" t="n"/>
+      <c r="K8" s="9" t="n"/>
+      <c r="L8" s="34" t="n"/>
     </row>
     <row customHeight="1" ht="77.25" r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="14" t="inlineStr">
+      <c r="B9" s="9" t="inlineStr">
         <is>
           <t>Santoshnagar-39</t>
         </is>
       </c>
-      <c r="C9" s="21" t="inlineStr">
+      <c r="C9" s="13" t="inlineStr">
         <is>
           <t>Rajesh &amp; 8074007813</t>
         </is>
@@ -1625,40 +1581,40 @@
       <c r="D9" s="3" t="n">
         <v>2.4</v>
       </c>
-      <c r="E9" s="21" t="inlineStr">
+      <c r="E9" s="13" t="inlineStr">
         <is>
           <t>Owasi Colony</t>
         </is>
       </c>
-      <c r="F9" s="1" t="inlineStr">
+      <c r="F9" s="33" t="inlineStr">
         <is>
           <t>Dasharath
 9652408382</t>
         </is>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="33" t="n">
         <v>2.2</v>
       </c>
-      <c r="H9" s="1" t="inlineStr">
+      <c r="H9" s="33" t="inlineStr">
         <is>
           <t>Kalendr Nagar</t>
         </is>
       </c>
-      <c r="I9" s="1" t="n"/>
-      <c r="J9" s="1" t="n"/>
-      <c r="K9" s="14" t="n"/>
-      <c r="L9" s="48" t="n"/>
+      <c r="I9" s="33" t="n"/>
+      <c r="J9" s="33" t="n"/>
+      <c r="K9" s="9" t="n"/>
+      <c r="L9" s="34" t="n"/>
     </row>
     <row customHeight="1" ht="106.5" r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="14" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>Talabchachlam-34</t>
         </is>
       </c>
-      <c r="C10" s="21" t="inlineStr">
+      <c r="C10" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">Md Mujeeb &amp; 8919569079 </t>
         </is>
@@ -1666,68 +1622,68 @@
       <c r="D10" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E10" s="21" t="inlineStr">
+      <c r="E10" s="13" t="inlineStr">
         <is>
           <t>Bhavani Nagar</t>
         </is>
       </c>
-      <c r="F10" s="1" t="inlineStr">
+      <c r="F10" s="33" t="inlineStr">
         <is>
           <t>Devender
 6281049862</t>
         </is>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H10" s="21" t="inlineStr">
+      <c r="H10" s="13" t="inlineStr">
         <is>
           <t>Bharani Nagar</t>
         </is>
       </c>
-      <c r="I10" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K10" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="48" t="n"/>
+      <c r="I10" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" s="34" t="n"/>
     </row>
     <row customHeight="1" ht="59.25" r="11">
-      <c r="A11" s="1" t="n"/>
-      <c r="B11" s="30" t="inlineStr">
+      <c r="A11" s="33" t="n"/>
+      <c r="B11" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C11" s="46" t="n"/>
-      <c r="D11" s="30">
+      <c r="C11" s="25" t="n"/>
+      <c r="D11" s="24">
         <f>SUM(D5:D10)</f>
         <v/>
       </c>
-      <c r="E11" s="1" t="n"/>
-      <c r="F11" s="1" t="n"/>
-      <c r="G11" s="33">
+      <c r="E11" s="33" t="n"/>
+      <c r="F11" s="33" t="n"/>
+      <c r="G11" s="30">
         <f>SUM(G5:G10)</f>
         <v/>
       </c>
-      <c r="H11" s="1" t="n"/>
-      <c r="I11" s="1" t="n"/>
-      <c r="J11" s="33">
+      <c r="H11" s="33" t="n"/>
+      <c r="I11" s="33" t="n"/>
+      <c r="J11" s="30">
         <f>SUM(J5:J10)</f>
         <v/>
       </c>
-      <c r="K11" s="1" t="n"/>
-      <c r="L11" s="47" t="n"/>
+      <c r="K11" s="33" t="n"/>
+      <c r="L11" s="31" t="n"/>
     </row>
     <row customHeight="1" ht="50.25" r="12"/>
     <row customHeight="1" ht="32.25" r="13"/>
@@ -1761,141 +1717,135 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="4.42578125"/>
-    <col customWidth="1" max="2" min="2" style="11" width="17.7109375"/>
-    <col customWidth="1" max="3" min="3" style="11" width="15.7109375"/>
-    <col customWidth="1" max="4" min="4" style="11" width="9.140625"/>
-    <col customWidth="1" max="9" min="5" style="11" width="14.140625"/>
-    <col customWidth="1" max="10" min="10" style="11" width="13.5703125"/>
-    <col customWidth="1" max="12" min="11" style="11" width="14.140625"/>
-    <col customWidth="1" max="16384" min="13" style="11" width="9.140625"/>
+    <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
+    <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
+    <col customWidth="1" max="3" min="3" style="29" width="15.7109375"/>
+    <col customWidth="1" max="4" min="4" style="29" width="9.140625"/>
+    <col customWidth="1" max="9" min="5" style="29" width="14.140625"/>
+    <col customWidth="1" max="10" min="10" style="29" width="13.5703125"/>
+    <col customWidth="1" max="12" min="11" style="29" width="14.140625"/>
+    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="28" t="inlineStr">
         <is>
           <t>GREATER HYDERABAD MUNICIPAL CORPORATION</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="45" r="2">
-      <c r="A2" s="11" t="n"/>
-      <c r="B2" s="31" t="inlineStr">
+      <c r="B2" s="26" t="inlineStr">
         <is>
           <t>Name of the Zone:Charminar Zone</t>
         </is>
       </c>
-      <c r="C2" s="31" t="n"/>
-      <c r="D2" s="11" t="n"/>
-      <c r="E2" s="11" t="n"/>
-      <c r="F2" s="11" t="n"/>
-      <c r="G2" s="11" t="n"/>
-      <c r="H2" s="11" t="n"/>
-      <c r="I2" s="11" t="n"/>
-      <c r="J2" s="6" t="inlineStr">
+      <c r="C2" s="26" t="n"/>
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Circle:8</t>
         </is>
       </c>
-      <c r="K2" s="31" t="inlineStr">
+      <c r="K2" s="26" t="inlineStr">
         <is>
           <t>Date:4.08.2020</t>
         </is>
       </c>
-      <c r="L2" s="31" t="n"/>
+      <c r="L2" s="26" t="n"/>
     </row>
     <row customHeight="1" ht="30" r="3">
-      <c r="A3" s="33" t="inlineStr">
+      <c r="A3" s="30" t="inlineStr">
         <is>
           <t>SL No</t>
         </is>
       </c>
-      <c r="B3" s="33" t="inlineStr">
+      <c r="B3" s="30" t="inlineStr">
         <is>
           <t>Division Name</t>
         </is>
       </c>
-      <c r="C3" s="33" t="inlineStr">
+      <c r="C3" s="30" t="inlineStr">
         <is>
           <t>PFM-1</t>
         </is>
       </c>
-      <c r="D3" s="33" t="n"/>
-      <c r="E3" s="33" t="n"/>
-      <c r="F3" s="33" t="inlineStr">
+      <c r="D3" s="30" t="n"/>
+      <c r="E3" s="30" t="n"/>
+      <c r="F3" s="30" t="inlineStr">
         <is>
           <t>PFM-2</t>
         </is>
       </c>
-      <c r="G3" s="33" t="n"/>
-      <c r="H3" s="33" t="n"/>
-      <c r="I3" s="33" t="inlineStr">
+      <c r="G3" s="30" t="n"/>
+      <c r="H3" s="30" t="n"/>
+      <c r="I3" s="30" t="inlineStr">
         <is>
           <t>VMF</t>
         </is>
       </c>
-      <c r="J3" s="33" t="n"/>
-      <c r="K3" s="33" t="n"/>
-      <c r="L3" s="33" t="n"/>
+      <c r="J3" s="30" t="n"/>
+      <c r="K3" s="30" t="n"/>
+      <c r="L3" s="30" t="n"/>
     </row>
     <row customHeight="1" ht="27.75" r="4">
-      <c r="A4" s="33" t="n"/>
-      <c r="B4" s="33" t="n"/>
-      <c r="C4" s="33" t="inlineStr">
+      <c r="A4" s="30" t="n"/>
+      <c r="B4" s="30" t="n"/>
+      <c r="C4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="D4" s="33" t="inlineStr">
+      <c r="D4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="E4" s="33" t="inlineStr">
+      <c r="E4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="F4" s="33" t="inlineStr">
+      <c r="F4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="G4" s="33" t="inlineStr">
+      <c r="G4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="H4" s="33" t="inlineStr">
+      <c r="H4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
+      <c r="I4" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">TL Name &amp; Mobile </t>
         </is>
       </c>
-      <c r="J4" s="33" t="inlineStr">
+      <c r="J4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="K4" s="33" t="inlineStr">
+      <c r="K4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="L4" s="33" t="inlineStr">
+      <c r="L4" s="30" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1903,7 +1853,7 @@
           <t>Lalithabagh-36</t>
         </is>
       </c>
-      <c r="C5" s="21" t="inlineStr">
+      <c r="C5" s="13" t="inlineStr">
         <is>
           <t>Shiva Prasad &amp;  9618632623</t>
         </is>
@@ -1911,46 +1861,46 @@
       <c r="D5" s="3" t="n">
         <v>2.4</v>
       </c>
-      <c r="E5" s="21" t="inlineStr">
+      <c r="E5" s="13" t="inlineStr">
         <is>
           <t>Jyothi Bhag</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="33" t="inlineStr">
         <is>
           <t>Masood 
 939841342</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H5" s="21" t="inlineStr">
+      <c r="H5" s="13" t="inlineStr">
         <is>
           <t>Vinayak Nagar</t>
         </is>
       </c>
-      <c r="I5" s="1" t="inlineStr">
+      <c r="I5" s="33" t="inlineStr">
         <is>
           <t>B Ramudu 8688749526</t>
         </is>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="J5" s="33" t="n">
         <v>17.5</v>
       </c>
-      <c r="K5" s="1" t="inlineStr">
+      <c r="K5" s="33" t="inlineStr">
         <is>
           <t>Narahari Nagar, Taraji Nagar, Maruti Nagar, Lalitabhag, Billa Nagar</t>
         </is>
       </c>
-      <c r="L5" s="1" t="inlineStr">
+      <c r="L5" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="60" r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -1958,7 +1908,7 @@
           <t>Riyasthnagar-40</t>
         </is>
       </c>
-      <c r="C6" s="21" t="inlineStr">
+      <c r="C6" s="13" t="inlineStr">
         <is>
           <t>N Shanker &amp; 9502763663</t>
         </is>
@@ -1966,45 +1916,45 @@
       <c r="D6" s="3" t="n">
         <v>2.3</v>
       </c>
-      <c r="E6" s="21" t="inlineStr">
+      <c r="E6" s="13" t="inlineStr">
         <is>
           <t>Jhamal Colony</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve">Md Rashed Khan
 9885242900
 </t>
         </is>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="33" t="n">
         <v>2.2</v>
       </c>
-      <c r="H6" s="21" t="inlineStr">
+      <c r="H6" s="13" t="inlineStr">
         <is>
           <t>Riyasath Nagar</t>
         </is>
       </c>
-      <c r="I6" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J6" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L6" s="1" t="n"/>
+      <c r="I6" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K6" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="92.25" r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -2012,7 +1962,7 @@
           <t>Kanchanbagh-41</t>
         </is>
       </c>
-      <c r="C7" s="21" t="inlineStr">
+      <c r="C7" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">V Bharath &amp; 8801113420 </t>
         </is>
@@ -2020,36 +1970,36 @@
       <c r="D7" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="21" t="inlineStr">
+      <c r="E7" s="13" t="inlineStr">
         <is>
           <t>A Block</t>
         </is>
       </c>
-      <c r="F7" s="1" t="inlineStr">
+      <c r="F7" s="33" t="inlineStr">
         <is>
           <t>D Ranganath
 9705882341</t>
         </is>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="33" t="n">
         <v>2.1</v>
       </c>
-      <c r="H7" s="1" t="inlineStr">
+      <c r="H7" s="33" t="inlineStr">
         <is>
           <t>C Block</t>
         </is>
       </c>
-      <c r="I7" s="1" t="n"/>
-      <c r="J7" s="1" t="n"/>
-      <c r="K7" s="13" t="n"/>
-      <c r="L7" s="1" t="inlineStr">
+      <c r="I7" s="33" t="n"/>
+      <c r="J7" s="33" t="n"/>
+      <c r="K7" s="8" t="n"/>
+      <c r="L7" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="88.5" r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -2057,7 +2007,7 @@
           <t>Barkas-42</t>
         </is>
       </c>
-      <c r="C8" s="21" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">Sathanarayana &amp; 7075705453 </t>
         </is>
@@ -2065,48 +2015,48 @@
       <c r="D8" s="3" t="n">
         <v>2.3</v>
       </c>
-      <c r="E8" s="1" t="inlineStr">
+      <c r="E8" s="33" t="inlineStr">
         <is>
           <t>Ahmad Nagar</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr">
+      <c r="F8" s="33" t="inlineStr">
         <is>
           <t>Narsing Rao
 7780669898</t>
         </is>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H8" s="1" t="inlineStr">
+      <c r="H8" s="33" t="inlineStr">
         <is>
           <t>Ram Nagar</t>
         </is>
       </c>
-      <c r="I8" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K8" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L8" s="1" t="inlineStr">
+      <c r="I8" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J8" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K8" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L8" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="65.25" r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -2114,7 +2064,7 @@
           <t>Chandryangutta-43</t>
         </is>
       </c>
-      <c r="C9" s="21" t="inlineStr">
+      <c r="C9" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">Shaik Nayeem &amp; 9989431803 </t>
         </is>
@@ -2122,47 +2072,47 @@
       <c r="D9" s="3" t="n">
         <v>2.7</v>
       </c>
-      <c r="E9" s="11" t="inlineStr">
+      <c r="E9" s="29" t="inlineStr">
         <is>
           <t>Babur Nagar B block</t>
         </is>
       </c>
-      <c r="F9" s="1" t="inlineStr">
+      <c r="F9" s="33" t="inlineStr">
         <is>
           <t>Jagan</t>
         </is>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H9" s="11" t="inlineStr">
+      <c r="H9" s="29" t="inlineStr">
         <is>
           <t>Bandlaguda</t>
         </is>
       </c>
-      <c r="I9" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K9" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L9" s="1" t="inlineStr">
+      <c r="I9" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J9" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K9" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L9" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="90.75" r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -2170,7 +2120,7 @@
           <t>Uppuguda-44</t>
         </is>
       </c>
-      <c r="C10" s="21" t="inlineStr">
+      <c r="C10" s="13" t="inlineStr">
         <is>
           <t>K Rakesh &amp; 9959636750</t>
         </is>
@@ -2178,47 +2128,47 @@
       <c r="D10" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E10" s="1" t="inlineStr">
+      <c r="E10" s="33" t="inlineStr">
         <is>
           <t>Shivaji Nagar</t>
         </is>
       </c>
-      <c r="F10" s="1" t="inlineStr">
+      <c r="F10" s="33" t="inlineStr">
         <is>
           <t>Rakesh 9959636750</t>
         </is>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="33" t="n">
         <v>2.3</v>
       </c>
-      <c r="H10" s="1" t="inlineStr">
+      <c r="H10" s="33" t="inlineStr">
         <is>
           <t>Mahankali Temple</t>
         </is>
       </c>
-      <c r="I10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J10" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="1" t="inlineStr">
+      <c r="I10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="102" r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="33" t="n">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -2226,7 +2176,7 @@
           <t>Jangammet-45</t>
         </is>
       </c>
-      <c r="C11" s="21" t="inlineStr">
+      <c r="C11" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">C Manhohar &amp; 9059930220 </t>
         </is>
@@ -2234,54 +2184,54 @@
       <c r="D11" s="3" t="n">
         <v>2.1</v>
       </c>
-      <c r="E11" s="21" t="inlineStr">
+      <c r="E11" s="13" t="inlineStr">
         <is>
           <t>Al Mustafa Colony</t>
         </is>
       </c>
-      <c r="F11" s="1" t="inlineStr">
+      <c r="F11" s="33" t="inlineStr">
         <is>
           <t>mahesh</t>
         </is>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="33" t="n">
         <v>2.1</v>
       </c>
-      <c r="H11" s="1" t="inlineStr">
+      <c r="H11" s="33" t="inlineStr">
         <is>
           <t>Kadri Chaman</t>
         </is>
       </c>
-      <c r="I11" s="1" t="n"/>
-      <c r="J11" s="1" t="n"/>
-      <c r="K11" s="13" t="n"/>
-      <c r="L11" s="1" t="n"/>
+      <c r="I11" s="33" t="n"/>
+      <c r="J11" s="33" t="n"/>
+      <c r="K11" s="8" t="n"/>
+      <c r="L11" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="50.25" r="12">
-      <c r="A12" s="1" t="n"/>
-      <c r="B12" s="30" t="inlineStr">
+      <c r="A12" s="33" t="n"/>
+      <c r="B12" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C12" s="46" t="n"/>
-      <c r="D12" s="30">
+      <c r="C12" s="25" t="n"/>
+      <c r="D12" s="24">
         <f>SUM(D5:D11)</f>
         <v/>
       </c>
-      <c r="E12" s="1" t="n"/>
-      <c r="F12" s="1" t="n"/>
-      <c r="G12" s="33">
+      <c r="E12" s="33" t="n"/>
+      <c r="F12" s="33" t="n"/>
+      <c r="G12" s="30">
         <f>SUM(G5:G11)</f>
         <v/>
       </c>
-      <c r="H12" s="1" t="n"/>
-      <c r="I12" s="1" t="n"/>
-      <c r="J12" s="33" t="n">
+      <c r="H12" s="33" t="n"/>
+      <c r="I12" s="33" t="n"/>
+      <c r="J12" s="30" t="n">
         <v>17.5</v>
       </c>
-      <c r="K12" s="1" t="n"/>
-      <c r="L12" s="1" t="n"/>
+      <c r="K12" s="33" t="n"/>
+      <c r="L12" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="87" r="13"/>
   </sheetData>
@@ -2306,147 +2256,141 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="4.42578125"/>
-    <col customWidth="1" max="2" min="2" style="11" width="17.7109375"/>
-    <col customWidth="1" max="3" min="3" style="11" width="15.7109375"/>
-    <col customWidth="1" max="4" min="4" style="11" width="9.140625"/>
-    <col customWidth="1" max="12" min="5" style="11" width="14.140625"/>
-    <col customWidth="1" max="16384" min="13" style="11" width="9.140625"/>
+    <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
+    <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
+    <col customWidth="1" max="3" min="3" style="29" width="15.7109375"/>
+    <col customWidth="1" max="4" min="4" style="29" width="9.140625"/>
+    <col customWidth="1" max="12" min="5" style="29" width="14.140625"/>
+    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="28" t="inlineStr">
         <is>
           <t>GREATER HYDERABAD MUNICIPAL CORPORATION</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="45" r="2">
-      <c r="A2" s="11" t="n"/>
-      <c r="B2" s="31" t="inlineStr">
+      <c r="B2" s="26" t="inlineStr">
         <is>
           <t>Name of the Zone:Charminar Zone</t>
         </is>
       </c>
-      <c r="C2" s="31" t="n"/>
-      <c r="D2" s="11" t="n"/>
-      <c r="E2" s="11" t="n"/>
-      <c r="F2" s="11" t="n"/>
-      <c r="G2" s="11" t="n"/>
-      <c r="H2" s="11" t="n"/>
-      <c r="I2" s="11" t="n"/>
-      <c r="J2" s="6" t="inlineStr">
+      <c r="C2" s="26" t="n"/>
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Circle:9</t>
         </is>
       </c>
-      <c r="K2" s="31" t="inlineStr">
+      <c r="K2" s="26" t="inlineStr">
         <is>
           <t>Date:4.08.2020</t>
         </is>
       </c>
-      <c r="L2" s="31" t="n"/>
+      <c r="L2" s="26" t="n"/>
     </row>
     <row customHeight="1" ht="27.75" r="3">
-      <c r="A3" s="33" t="inlineStr">
+      <c r="A3" s="30" t="inlineStr">
         <is>
           <t>SL No</t>
         </is>
       </c>
-      <c r="B3" s="33" t="inlineStr">
+      <c r="B3" s="30" t="inlineStr">
         <is>
           <t>Division Name</t>
         </is>
       </c>
-      <c r="C3" s="33" t="inlineStr">
+      <c r="C3" s="30" t="inlineStr">
         <is>
           <t>PFM-1</t>
         </is>
       </c>
-      <c r="D3" s="33" t="n"/>
-      <c r="E3" s="33" t="n"/>
-      <c r="F3" s="33" t="inlineStr">
+      <c r="D3" s="30" t="n"/>
+      <c r="E3" s="30" t="n"/>
+      <c r="F3" s="30" t="inlineStr">
         <is>
           <t>PFM-2</t>
         </is>
       </c>
-      <c r="G3" s="33" t="n"/>
-      <c r="H3" s="33" t="n"/>
-      <c r="I3" s="33" t="inlineStr">
+      <c r="G3" s="30" t="n"/>
+      <c r="H3" s="30" t="n"/>
+      <c r="I3" s="30" t="inlineStr">
         <is>
           <t>VMF</t>
         </is>
       </c>
-      <c r="J3" s="33" t="n"/>
-      <c r="K3" s="33" t="n"/>
-      <c r="L3" s="33" t="n"/>
+      <c r="J3" s="30" t="n"/>
+      <c r="K3" s="30" t="n"/>
+      <c r="L3" s="30" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="4">
-      <c r="A4" s="33" t="n"/>
-      <c r="B4" s="33" t="n"/>
-      <c r="C4" s="33" t="inlineStr">
+      <c r="A4" s="30" t="n"/>
+      <c r="B4" s="30" t="n"/>
+      <c r="C4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="D4" s="33" t="inlineStr">
+      <c r="D4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="E4" s="33" t="inlineStr">
+      <c r="E4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="F4" s="33" t="inlineStr">
+      <c r="F4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="G4" s="33" t="inlineStr">
+      <c r="G4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="H4" s="33" t="inlineStr">
+      <c r="H4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
+      <c r="I4" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">TL Name &amp; Mobile </t>
         </is>
       </c>
-      <c r="J4" s="33" t="inlineStr">
+      <c r="J4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="K4" s="33" t="inlineStr">
+      <c r="K4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="L4" s="33" t="inlineStr">
+      <c r="L4" s="30" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="30" r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Pathergatti-32</t>
         </is>
       </c>
-      <c r="C5" s="21" t="inlineStr">
+      <c r="C5" s="13" t="inlineStr">
         <is>
           <t>Shiva &amp;  9502535493</t>
         </is>
@@ -2454,56 +2398,56 @@
       <c r="D5" s="3" t="n">
         <v>2.2</v>
       </c>
-      <c r="E5" s="21" t="inlineStr">
+      <c r="E5" s="13" t="inlineStr">
         <is>
           <t>Unani Hospital</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="33" t="inlineStr">
         <is>
           <t>Shayam
 9121796153</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H5" s="1" t="inlineStr">
+      <c r="H5" s="33" t="inlineStr">
         <is>
           <t>Pather Ghati</t>
         </is>
       </c>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="inlineStr">
+      <c r="I5" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J5" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K5" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="30" r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Shalibanda-48</t>
         </is>
       </c>
-      <c r="C6" s="21" t="inlineStr">
+      <c r="C6" s="13" t="inlineStr">
         <is>
           <t>Ali baba &amp; 8328654875</t>
         </is>
@@ -2511,56 +2455,56 @@
       <c r="D6" s="3" t="n">
         <v>2.4</v>
       </c>
-      <c r="E6" s="21" t="inlineStr">
+      <c r="E6" s="13" t="inlineStr">
         <is>
           <t>Khaji Pura</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="33" t="inlineStr">
         <is>
           <t>A Mahender
 9177396155</t>
         </is>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="33" t="n">
         <v>2.2</v>
       </c>
-      <c r="H6" s="1" t="inlineStr">
+      <c r="H6" s="33" t="inlineStr">
         <is>
           <t>Budhri Halwa</t>
         </is>
       </c>
-      <c r="I6" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L6" s="1" t="inlineStr">
+      <c r="I6" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J6" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K6" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="30" r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>Puranapul-52</t>
         </is>
       </c>
-      <c r="C7" s="21" t="inlineStr">
+      <c r="C7" s="13" t="inlineStr">
         <is>
           <t>MD Majid &amp; 7780173117</t>
         </is>
@@ -2568,56 +2512,56 @@
       <c r="D7" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="21" t="inlineStr">
+      <c r="E7" s="13" t="inlineStr">
         <is>
           <t>Aligulsham</t>
         </is>
       </c>
-      <c r="F7" s="1" t="inlineStr">
+      <c r="F7" s="33" t="inlineStr">
         <is>
           <t>Faqruddin
 9396439208</t>
         </is>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="33" t="n">
         <v>2.3</v>
       </c>
-      <c r="H7" s="1" t="inlineStr">
+      <c r="H7" s="33" t="inlineStr">
         <is>
           <t>Tara Mandir</t>
         </is>
       </c>
-      <c r="I7" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L7" s="1" t="inlineStr">
+      <c r="I7" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J7" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K7" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L7" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="30" r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>Moghalpura-33</t>
         </is>
       </c>
-      <c r="C8" s="21" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">Kirankuamar &amp; 9398465271 </t>
         </is>
@@ -2625,48 +2569,47 @@
       <c r="D8" s="3" t="n">
         <v>2.6</v>
       </c>
-      <c r="E8" s="21" t="inlineStr">
+      <c r="E8" s="13" t="inlineStr">
         <is>
           <t>Moghalpura Water Tank</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr">
+      <c r="F8" s="33" t="inlineStr">
         <is>
           <t>Srinivas
 9390770911</t>
         </is>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H8" s="21" t="inlineStr">
+      <c r="H8" s="13" t="inlineStr">
         <is>
           <t>Billa Colony</t>
         </is>
       </c>
-      <c r="I8" s="11" t="n"/>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K8" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L8" s="1" t="n"/>
+      <c r="J8" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K8" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L8" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="90" r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>Ghansibazar-49</t>
         </is>
       </c>
-      <c r="C9" s="21" t="inlineStr">
+      <c r="C9" s="13" t="inlineStr">
         <is>
           <t>Bikshapathi &amp;  6302782341</t>
         </is>
@@ -2674,71 +2617,71 @@
       <c r="D9" s="3" t="n">
         <v>2.1</v>
       </c>
-      <c r="E9" s="21" t="inlineStr">
+      <c r="E9" s="13" t="inlineStr">
         <is>
           <t>Husain Alam</t>
         </is>
       </c>
-      <c r="F9" s="19" t="inlineStr">
+      <c r="F9" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">Arjun
 8801838776
 </t>
         </is>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H9" s="21" t="inlineStr">
+      <c r="H9" s="13" t="inlineStr">
         <is>
           <t>Musa Bowli</t>
         </is>
       </c>
-      <c r="I9" s="1" t="inlineStr">
+      <c r="I9" s="33" t="inlineStr">
         <is>
           <t>Jatavath Swamy
 9640788116</t>
         </is>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="J9" s="33" t="n">
         <v>17</v>
       </c>
-      <c r="K9" s="1" t="inlineStr">
+      <c r="K9" s="33" t="inlineStr">
         <is>
           <t>Doodh Bowli, Ghanji Bazar, Guljar House, Charkham Charimnar bandi ka adda</t>
         </is>
       </c>
-      <c r="L9" s="1" t="inlineStr">
+      <c r="L9" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="10">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="30" t="inlineStr">
+      <c r="A10" s="33" t="n"/>
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C10" s="46" t="n"/>
-      <c r="D10" s="30">
+      <c r="C10" s="25" t="n"/>
+      <c r="D10" s="24">
         <f>SUM(D5:D9)</f>
         <v/>
       </c>
-      <c r="E10" s="1" t="n"/>
-      <c r="F10" s="1" t="n"/>
-      <c r="G10" s="33">
+      <c r="E10" s="33" t="n"/>
+      <c r="F10" s="33" t="n"/>
+      <c r="G10" s="30">
         <f>SUM(G5:G9)</f>
         <v/>
       </c>
-      <c r="H10" s="1" t="n"/>
-      <c r="I10" s="1" t="n"/>
-      <c r="J10" s="33" t="n">
+      <c r="H10" s="33" t="n"/>
+      <c r="I10" s="33" t="n"/>
+      <c r="J10" s="30" t="n">
         <v>17</v>
       </c>
-      <c r="K10" s="1" t="n"/>
-      <c r="L10" s="1" t="n"/>
+      <c r="K10" s="33" t="n"/>
+      <c r="L10" s="33" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2762,149 +2705,143 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="4.42578125"/>
-    <col customWidth="1" max="2" min="2" style="11" width="17.7109375"/>
-    <col customWidth="1" max="3" min="3" style="11" width="15.7109375"/>
-    <col customWidth="1" max="4" min="4" style="11" width="9.140625"/>
-    <col customWidth="1" max="10" min="5" style="11" width="14.140625"/>
-    <col customWidth="1" max="11" min="11" style="11" width="19"/>
-    <col customWidth="1" max="12" min="12" style="11" width="14.140625"/>
-    <col customWidth="1" max="16384" min="13" style="11" width="9.140625"/>
+    <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
+    <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
+    <col customWidth="1" max="3" min="3" style="29" width="15.7109375"/>
+    <col customWidth="1" max="4" min="4" style="29" width="9.140625"/>
+    <col customWidth="1" max="10" min="5" style="29" width="14.140625"/>
+    <col customWidth="1" max="11" min="11" style="29" width="19"/>
+    <col customWidth="1" max="12" min="12" style="29" width="14.140625"/>
+    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="28" t="inlineStr">
         <is>
           <t>GREATER HYDERABAD MUNICIPAL CORPORATION</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2">
-      <c r="A2" s="11" t="n"/>
-      <c r="B2" s="31" t="inlineStr">
+      <c r="B2" s="26" t="inlineStr">
         <is>
           <t>Name of the Zone:Charminar Zone</t>
         </is>
       </c>
-      <c r="C2" s="44" t="n"/>
-      <c r="D2" s="11" t="n"/>
-      <c r="E2" s="11" t="n"/>
-      <c r="F2" s="11" t="n"/>
-      <c r="G2" s="11" t="n"/>
-      <c r="H2" s="11" t="n"/>
-      <c r="I2" s="11" t="n"/>
-      <c r="J2" s="6" t="inlineStr">
+      <c r="C2" s="27" t="n"/>
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Circle:10</t>
         </is>
       </c>
-      <c r="K2" s="31" t="inlineStr">
+      <c r="K2" s="26" t="inlineStr">
         <is>
           <t>Date:4.08.2020</t>
         </is>
       </c>
-      <c r="L2" s="44" t="n"/>
+      <c r="L2" s="27" t="n"/>
     </row>
     <row customHeight="1" ht="30.75" r="3">
-      <c r="A3" s="39" t="inlineStr">
+      <c r="A3" s="19" t="inlineStr">
         <is>
           <t>SL No</t>
         </is>
       </c>
-      <c r="B3" s="39" t="inlineStr">
+      <c r="B3" s="19" t="inlineStr">
         <is>
           <t>Division Name</t>
         </is>
       </c>
-      <c r="C3" s="40" t="inlineStr">
+      <c r="C3" s="20" t="inlineStr">
         <is>
           <t>PFM-1</t>
         </is>
       </c>
-      <c r="D3" s="41" t="n"/>
-      <c r="E3" s="42" t="n"/>
-      <c r="F3" s="40" t="inlineStr">
+      <c r="D3" s="21" t="n"/>
+      <c r="E3" s="22" t="n"/>
+      <c r="F3" s="20" t="inlineStr">
         <is>
           <t>PFM-2</t>
         </is>
       </c>
-      <c r="G3" s="41" t="n"/>
-      <c r="H3" s="42" t="n"/>
-      <c r="I3" s="40" t="inlineStr">
+      <c r="G3" s="21" t="n"/>
+      <c r="H3" s="22" t="n"/>
+      <c r="I3" s="20" t="inlineStr">
         <is>
           <t>VMF</t>
         </is>
       </c>
-      <c r="J3" s="41" t="n"/>
-      <c r="K3" s="42" t="n"/>
-      <c r="L3" s="33" t="n"/>
+      <c r="J3" s="21" t="n"/>
+      <c r="K3" s="22" t="n"/>
+      <c r="L3" s="30" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="4">
-      <c r="A4" s="43" t="n"/>
-      <c r="B4" s="43" t="n"/>
-      <c r="C4" s="33" t="inlineStr">
+      <c r="A4" s="23" t="n"/>
+      <c r="B4" s="23" t="n"/>
+      <c r="C4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="D4" s="33" t="inlineStr">
+      <c r="D4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="E4" s="33" t="inlineStr">
+      <c r="E4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="F4" s="33" t="inlineStr">
+      <c r="F4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="G4" s="33" t="inlineStr">
+      <c r="G4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="H4" s="33" t="inlineStr">
+      <c r="H4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
+      <c r="I4" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">TL Name &amp; Mobile </t>
         </is>
       </c>
-      <c r="J4" s="33" t="inlineStr">
+      <c r="J4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="K4" s="33" t="inlineStr">
+      <c r="K4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="L4" s="33" t="inlineStr">
+      <c r="L4" s="30" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="60" r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Dhood Bowli-53</t>
         </is>
       </c>
-      <c r="C5" s="21" t="inlineStr">
+      <c r="C5" s="13" t="inlineStr">
         <is>
           <t>Md Riyaz &amp; 9398135298</t>
         </is>
@@ -2912,54 +2849,54 @@
       <c r="D5" s="3" t="n">
         <v>2.6</v>
       </c>
-      <c r="E5" s="21" t="inlineStr">
+      <c r="E5" s="13" t="inlineStr">
         <is>
           <t>Fathedharwasa</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="33" t="inlineStr">
         <is>
           <t>MD Raoof
 9502235275</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H5" s="1" t="inlineStr">
+      <c r="H5" s="33" t="inlineStr">
         <is>
           <t>Moinpura</t>
         </is>
       </c>
-      <c r="I5" s="1" t="inlineStr">
+      <c r="I5" s="33" t="inlineStr">
         <is>
           <t>Osman 9550442587</t>
         </is>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="J5" s="33" t="n">
         <v>18.5</v>
       </c>
-      <c r="K5" s="1" t="inlineStr">
+      <c r="K5" s="33" t="inlineStr">
         <is>
           <t>Gollahkidiki, Moorali Nagar, Maharaj Ganj, Palam Road</t>
         </is>
       </c>
-      <c r="L5" s="1" t="inlineStr">
+      <c r="L5" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="121.5" r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Ramnaspura-55</t>
         </is>
       </c>
-      <c r="C6" s="21" t="inlineStr">
+      <c r="C6" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">MD Waseem &amp; 8801984231 </t>
         </is>
@@ -2967,40 +2904,40 @@
       <c r="D6" s="3" t="n">
         <v>2.2</v>
       </c>
-      <c r="E6" s="21" t="inlineStr">
+      <c r="E6" s="13" t="inlineStr">
         <is>
           <t>Khaja Pahadi</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="33" t="inlineStr">
         <is>
           <t>U Ganesh
 9989784005</t>
         </is>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="33" t="n">
         <v>2.1</v>
       </c>
-      <c r="H6" s="1" t="inlineStr">
+      <c r="H6" s="33" t="inlineStr">
         <is>
           <t>Ramanaspura</t>
         </is>
       </c>
-      <c r="I6" s="1" t="n"/>
-      <c r="J6" s="1" t="n"/>
-      <c r="K6" s="1" t="n"/>
-      <c r="L6" s="1" t="n"/>
+      <c r="I6" s="33" t="n"/>
+      <c r="J6" s="33" t="n"/>
+      <c r="K6" s="33" t="n"/>
+      <c r="L6" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="30" r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>Jahanuma-54</t>
         </is>
       </c>
-      <c r="C7" s="21" t="inlineStr">
+      <c r="C7" s="13" t="inlineStr">
         <is>
           <t>Jagdishwaer &amp; 9533744179</t>
         </is>
@@ -3008,56 +2945,56 @@
       <c r="D7" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="21" t="inlineStr">
+      <c r="E7" s="13" t="inlineStr">
         <is>
           <t>Pulbhag</t>
         </is>
       </c>
-      <c r="F7" s="1" t="inlineStr">
+      <c r="F7" s="33" t="inlineStr">
         <is>
           <t>P Jangaiah
 8074602806</t>
         </is>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="33" t="n">
         <v>2.2</v>
       </c>
-      <c r="H7" s="1" t="inlineStr">
+      <c r="H7" s="33" t="inlineStr">
         <is>
           <t>Jahanuma</t>
         </is>
       </c>
-      <c r="I7" s="28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K7" s="29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L7" s="1" t="inlineStr">
+      <c r="I7" s="14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J7" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K7" s="15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L7" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="106.5" r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>Kishanbagh-56</t>
         </is>
       </c>
-      <c r="C8" s="21" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t>Mahender &amp; 9700705283</t>
         </is>
@@ -3065,39 +3002,37 @@
       <c r="D8" s="3" t="n">
         <v>2.2</v>
       </c>
-      <c r="E8" s="1" t="inlineStr">
+      <c r="E8" s="33" t="inlineStr">
         <is>
           <t>Allah Masjid</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr">
+      <c r="F8" s="33" t="inlineStr">
         <is>
           <t>Mustafa</t>
         </is>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H8" s="21" t="inlineStr">
+      <c r="H8" s="13" t="inlineStr">
         <is>
           <t>Kishanbhagh</t>
         </is>
       </c>
-      <c r="I8" s="11" t="n"/>
-      <c r="J8" s="1" t="n"/>
-      <c r="K8" s="11" t="n"/>
-      <c r="L8" s="1" t="n"/>
+      <c r="J8" s="33" t="n"/>
+      <c r="L8" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="110.25" r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>Nawabshab Kunta-47</t>
         </is>
       </c>
-      <c r="C9" s="21" t="inlineStr">
+      <c r="C9" s="13" t="inlineStr">
         <is>
           <t>Arjun &amp; 8501890109</t>
         </is>
@@ -3105,118 +3040,118 @@
       <c r="D9" s="3" t="n">
         <v>2.3</v>
       </c>
-      <c r="E9" s="21" t="inlineStr">
+      <c r="E9" s="13" t="inlineStr">
         <is>
           <t>Janumalalsar</t>
         </is>
       </c>
-      <c r="F9" s="1" t="inlineStr">
+      <c r="F9" s="33" t="inlineStr">
         <is>
           <t>Mothilal 9912246042</t>
         </is>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H9" s="21" t="inlineStr">
+      <c r="H9" s="13" t="inlineStr">
         <is>
           <t>Sanjay Gandhi nagar</t>
         </is>
       </c>
-      <c r="I9" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K9" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L9" s="1" t="n"/>
+      <c r="I9" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J9" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K9" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L9" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="30" r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>Falaknuma-46</t>
         </is>
       </c>
-      <c r="C10" s="21" t="inlineStr">
+      <c r="C10" s="13" t="inlineStr">
         <is>
           <t>S Raju &amp;  9440993466</t>
         </is>
       </c>
-      <c r="D10" s="21" t="n">
+      <c r="D10" s="13" t="n">
         <v>2.2</v>
       </c>
-      <c r="E10" s="21" t="inlineStr">
+      <c r="E10" s="13" t="inlineStr">
         <is>
           <t>Aljabal Colony</t>
         </is>
       </c>
-      <c r="F10" s="1" t="inlineStr">
+      <c r="F10" s="33" t="inlineStr">
         <is>
           <t>Naresh 7989189271</t>
         </is>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H10" s="1" t="inlineStr">
+      <c r="H10" s="33" t="inlineStr">
         <is>
           <t>Falaknuma</t>
         </is>
       </c>
-      <c r="I10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="1" t="n"/>
+      <c r="I10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="11">
-      <c r="A11" s="1" t="n"/>
-      <c r="B11" s="30" t="inlineStr">
+      <c r="A11" s="33" t="n"/>
+      <c r="B11" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C11" s="46" t="n"/>
-      <c r="D11" s="30">
+      <c r="C11" s="25" t="n"/>
+      <c r="D11" s="24">
         <f>SUM(D5:D10)</f>
         <v/>
       </c>
-      <c r="E11" s="1" t="n"/>
-      <c r="F11" s="1" t="n"/>
-      <c r="G11" s="33">
+      <c r="E11" s="33" t="n"/>
+      <c r="F11" s="33" t="n"/>
+      <c r="G11" s="30">
         <f>SUM(G5:G10)</f>
         <v/>
       </c>
-      <c r="H11" s="1" t="n"/>
-      <c r="I11" s="1" t="n"/>
-      <c r="J11" s="33" t="n">
+      <c r="H11" s="33" t="n"/>
+      <c r="I11" s="33" t="n"/>
+      <c r="J11" s="30" t="n">
         <v>18.5</v>
       </c>
-      <c r="K11" s="1" t="n"/>
-      <c r="L11" s="1" t="n"/>
+      <c r="K11" s="33" t="n"/>
+      <c r="L11" s="33" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3242,140 +3177,134 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="4.42578125"/>
-    <col customWidth="1" max="2" min="2" style="11" width="17.7109375"/>
-    <col customWidth="1" max="3" min="3" style="11" width="15.7109375"/>
-    <col customWidth="1" max="4" min="4" style="11" width="9.140625"/>
-    <col customWidth="1" max="5" min="5" style="11" width="14.7109375"/>
-    <col customWidth="1" max="6" min="6" style="11" width="14.140625"/>
-    <col customWidth="1" max="7" min="7" style="11" width="11.28515625"/>
-    <col customWidth="1" max="8" min="8" style="11" width="16.5703125"/>
-    <col customWidth="1" max="12" min="9" style="11" width="14.140625"/>
-    <col customWidth="1" max="16384" min="13" style="11" width="9.140625"/>
+    <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
+    <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
+    <col customWidth="1" max="3" min="3" style="29" width="15.7109375"/>
+    <col customWidth="1" max="4" min="4" style="29" width="9.140625"/>
+    <col customWidth="1" max="5" min="5" style="29" width="14.7109375"/>
+    <col customWidth="1" max="6" min="6" style="29" width="14.140625"/>
+    <col customWidth="1" max="7" min="7" style="29" width="11.28515625"/>
+    <col customWidth="1" max="8" min="8" style="29" width="16.5703125"/>
+    <col customWidth="1" max="12" min="9" style="29" width="14.140625"/>
+    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
-      <c r="A1" s="32" t="inlineStr">
+      <c r="A1" s="28" t="inlineStr">
         <is>
           <t>GREATER HYDERABAD MUNICIPAL CORPORATION</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="45" r="2">
-      <c r="B2" s="31" t="inlineStr">
+      <c r="B2" s="26" t="inlineStr">
         <is>
           <t>Name of the Zone:Charminar Zone</t>
         </is>
       </c>
-      <c r="C2" s="31" t="n"/>
-      <c r="D2" s="11" t="n"/>
-      <c r="E2" s="11" t="n"/>
-      <c r="F2" s="11" t="n"/>
-      <c r="G2" s="11" t="n"/>
-      <c r="H2" s="11" t="n"/>
-      <c r="I2" s="11" t="n"/>
-      <c r="J2" s="6" t="inlineStr">
+      <c r="C2" s="26" t="n"/>
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Circle:11</t>
         </is>
       </c>
-      <c r="K2" s="31" t="inlineStr">
+      <c r="K2" s="26" t="inlineStr">
         <is>
           <t>Date:4.08.2020</t>
         </is>
       </c>
-      <c r="L2" s="31" t="n"/>
+      <c r="L2" s="26" t="n"/>
     </row>
     <row r="3">
-      <c r="B3" s="39" t="inlineStr">
+      <c r="B3" s="19" t="inlineStr">
         <is>
           <t>Division Name</t>
         </is>
       </c>
-      <c r="C3" s="40" t="inlineStr">
+      <c r="C3" s="20" t="inlineStr">
         <is>
           <t>PFM-1</t>
         </is>
       </c>
-      <c r="D3" s="41" t="n"/>
-      <c r="E3" s="42" t="n"/>
-      <c r="F3" s="40" t="inlineStr">
+      <c r="D3" s="21" t="n"/>
+      <c r="E3" s="22" t="n"/>
+      <c r="F3" s="20" t="inlineStr">
         <is>
           <t>PFM-2</t>
         </is>
       </c>
-      <c r="G3" s="41" t="n"/>
-      <c r="H3" s="42" t="n"/>
-      <c r="I3" s="40" t="inlineStr">
+      <c r="G3" s="21" t="n"/>
+      <c r="H3" s="22" t="n"/>
+      <c r="I3" s="20" t="inlineStr">
         <is>
           <t>VMF</t>
         </is>
       </c>
-      <c r="J3" s="41" t="n"/>
-      <c r="K3" s="42" t="n"/>
-      <c r="L3" s="33" t="n"/>
+      <c r="J3" s="21" t="n"/>
+      <c r="K3" s="22" t="n"/>
+      <c r="L3" s="30" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="4">
-      <c r="B4" s="43" t="n"/>
-      <c r="C4" s="33" t="inlineStr">
+      <c r="B4" s="23" t="n"/>
+      <c r="C4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="D4" s="33" t="inlineStr">
+      <c r="D4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="E4" s="33" t="inlineStr">
+      <c r="E4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="F4" s="33" t="inlineStr">
+      <c r="F4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
         </is>
       </c>
-      <c r="G4" s="33" t="n">
+      <c r="G4" s="30" t="n">
         <v>2.5</v>
       </c>
-      <c r="H4" s="33" t="inlineStr">
+      <c r="H4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
+      <c r="I4" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">TL Name &amp; Mobile </t>
         </is>
       </c>
-      <c r="J4" s="33" t="inlineStr">
+      <c r="J4" s="30" t="inlineStr">
         <is>
           <t>KMs Covered</t>
         </is>
       </c>
-      <c r="K4" s="33" t="inlineStr">
+      <c r="K4" s="30" t="inlineStr">
         <is>
           <t>Areas Covered</t>
         </is>
       </c>
-      <c r="L4" s="33" t="inlineStr">
+      <c r="L4" s="30" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="34.5" r="5">
-      <c r="A5" s="11" t="n"/>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Suleman nagar-57</t>
         </is>
       </c>
-      <c r="C5" s="21" t="inlineStr">
+      <c r="C5" s="13" t="inlineStr">
         <is>
           <t>K Suresh Kumar &amp; 9848486473</t>
         </is>
@@ -3383,46 +3312,46 @@
       <c r="D5" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E5" s="21" t="inlineStr">
+      <c r="E5" s="13" t="inlineStr">
         <is>
           <t>Koi Muhamad</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="33" t="inlineStr">
         <is>
           <t>G Krishna
 9391138587</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="33" t="n">
         <v>2.1</v>
       </c>
-      <c r="H5" s="1" t="inlineStr">
+      <c r="H5" s="33" t="inlineStr">
         <is>
           <t>MM Pahadi</t>
         </is>
       </c>
-      <c r="I5" s="1" t="n"/>
-      <c r="J5" s="1" t="n"/>
-      <c r="K5" s="1" t="n"/>
-      <c r="L5" s="1" t="inlineStr">
+      <c r="I5" s="33" t="n"/>
+      <c r="J5" s="33" t="n"/>
+      <c r="K5" s="33" t="n"/>
+      <c r="L5" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15" r="6">
-      <c r="A6" s="33" t="inlineStr">
+      <c r="A6" s="30" t="inlineStr">
         <is>
           <t>SL No</t>
         </is>
       </c>
-      <c r="B6" s="7" t="inlineStr">
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>Shastripuram-58</t>
         </is>
       </c>
-      <c r="C6" s="21" t="inlineStr">
+      <c r="C6" s="13" t="inlineStr">
         <is>
           <t>M Vishnuvardhan &amp; 9700286845</t>
         </is>
@@ -3430,53 +3359,53 @@
       <c r="D6" s="3" t="n">
         <v>2.4</v>
       </c>
-      <c r="E6" s="21" t="inlineStr">
+      <c r="E6" s="13" t="inlineStr">
         <is>
           <t>Ashan Nagar</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="33" t="inlineStr">
         <is>
           <t>Hanumaiah
 9059190938</t>
         </is>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H6" s="21" t="inlineStr">
+      <c r="H6" s="13" t="inlineStr">
         <is>
           <t>Owasi Hills</t>
         </is>
       </c>
-      <c r="I6" s="1" t="inlineStr">
+      <c r="I6" s="33" t="inlineStr">
         <is>
           <t>S Prashanthraj
 9398651412</t>
         </is>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="J6" s="33" t="n">
         <v>17</v>
       </c>
-      <c r="K6" s="13" t="inlineStr">
+      <c r="K6" s="8" t="inlineStr">
         <is>
           <t>BK puram, Vattapalli, Shasthri Puram</t>
         </is>
       </c>
-      <c r="L6" s="1" t="inlineStr">
+      <c r="L6" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="36" r="7">
-      <c r="A7" s="47" t="n"/>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="A7" s="31" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>Mailerdevpally-59</t>
         </is>
       </c>
-      <c r="C7" s="21" t="inlineStr">
+      <c r="C7" s="13" t="inlineStr">
         <is>
           <t>K Vinod Kumar &amp; 8309606521</t>
         </is>
@@ -3484,44 +3413,44 @@
       <c r="D7" s="3" t="n">
         <v>2.2</v>
       </c>
-      <c r="E7" s="21" t="inlineStr">
+      <c r="E7" s="13" t="inlineStr">
         <is>
           <t>Aaranghar</t>
         </is>
       </c>
-      <c r="F7" s="1" t="inlineStr">
+      <c r="F7" s="33" t="inlineStr">
         <is>
           <t>Bhaskar
 7793966696</t>
         </is>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H7" s="21" t="inlineStr">
+      <c r="H7" s="13" t="inlineStr">
         <is>
           <t>NTR nagar</t>
         </is>
       </c>
-      <c r="I7" s="1" t="n"/>
-      <c r="J7" s="1" t="n"/>
-      <c r="K7" s="1" t="n"/>
-      <c r="L7" s="1" t="inlineStr">
+      <c r="I7" s="33" t="n"/>
+      <c r="J7" s="33" t="n"/>
+      <c r="K7" s="33" t="n"/>
+      <c r="L7" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="103.5" r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>Rajendranagar-60</t>
         </is>
       </c>
-      <c r="C8" s="21" t="inlineStr">
+      <c r="C8" s="13" t="inlineStr">
         <is>
           <t>Y Gopal &amp; 9346854806</t>
         </is>
@@ -3529,44 +3458,44 @@
       <c r="D8" s="3" t="n">
         <v>2.6</v>
       </c>
-      <c r="E8" s="21" t="inlineStr">
+      <c r="E8" s="13" t="inlineStr">
         <is>
           <t>Yadav Reddy Nagar</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr">
+      <c r="F8" s="33" t="inlineStr">
         <is>
           <t>Dhanraj
 9550258216</t>
         </is>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H8" s="21" t="inlineStr">
+      <c r="H8" s="13" t="inlineStr">
         <is>
           <t>Uppar Palli</t>
         </is>
       </c>
-      <c r="I8" s="1" t="n"/>
-      <c r="J8" s="1" t="n"/>
-      <c r="K8" s="1" t="n"/>
-      <c r="L8" s="1" t="inlineStr">
+      <c r="I8" s="33" t="n"/>
+      <c r="J8" s="33" t="n"/>
+      <c r="K8" s="33" t="n"/>
+      <c r="L8" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="90" r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>Attapur-61</t>
         </is>
       </c>
-      <c r="C9" s="21" t="inlineStr">
+      <c r="C9" s="13" t="inlineStr">
         <is>
           <t>Hyder guda</t>
         </is>
@@ -3574,55 +3503,55 @@
       <c r="D9" s="3" t="n">
         <v>2.4</v>
       </c>
-      <c r="E9" s="21" t="inlineStr">
+      <c r="E9" s="13" t="inlineStr">
         <is>
           <t>Khaj Nagar</t>
         </is>
       </c>
-      <c r="F9" s="1" t="inlineStr">
+      <c r="F9" s="33" t="inlineStr">
         <is>
           <t>Shamsunder
 8125247675</t>
         </is>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H9" s="21" t="inlineStr">
+      <c r="H9" s="13" t="inlineStr">
         <is>
           <t>Bharat Nagar</t>
         </is>
       </c>
-      <c r="I9" s="18" t="inlineStr">
+      <c r="I9" s="11" t="inlineStr">
         <is>
           <t>Ravi
 6302097148</t>
         </is>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="J9" s="33" t="n">
         <v>18.5</v>
       </c>
-      <c r="K9" s="13" t="inlineStr">
+      <c r="K9" s="8" t="inlineStr">
         <is>
           <t>Attapur Daltha Basthi, Bhagi Nagar, Indra Nagar, Tejeshwini colony</t>
         </is>
       </c>
-      <c r="L9" s="1" t="inlineStr">
+      <c r="L9" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="36" r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>Complaint Machine</t>
         </is>
       </c>
-      <c r="C10" s="21" t="inlineStr">
+      <c r="C10" s="13" t="inlineStr">
         <is>
           <t>Shyamsunder &amp; 8125247675</t>
         </is>
@@ -3630,84 +3559,84 @@
       <c r="D10" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E10" s="21" t="inlineStr">
+      <c r="E10" s="13" t="inlineStr">
         <is>
           <t>Rhagavendra Nagar</t>
         </is>
       </c>
-      <c r="F10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H10" s="1" t="n"/>
-      <c r="I10" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K10" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="1" t="inlineStr">
+      <c r="F10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" s="33" t="n"/>
+      <c r="I10" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" s="33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" s="33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="30" t="inlineStr">
+      <c r="B11" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C11" s="46" t="n"/>
-      <c r="D11" s="30">
+      <c r="C11" s="25" t="n"/>
+      <c r="D11" s="24">
         <f>SUM(D5:D10)</f>
         <v/>
       </c>
-      <c r="E11" s="1" t="n"/>
-      <c r="F11" s="1" t="n"/>
-      <c r="G11" s="30">
+      <c r="E11" s="33" t="n"/>
+      <c r="F11" s="33" t="n"/>
+      <c r="G11" s="24">
         <f>SUM(G5:G10)</f>
         <v/>
       </c>
-      <c r="H11" s="1" t="n"/>
-      <c r="I11" s="1" t="n"/>
-      <c r="J11" s="33">
+      <c r="H11" s="33" t="n"/>
+      <c r="I11" s="33" t="n"/>
+      <c r="J11" s="30">
         <f>SUM(J6:J10)</f>
         <v/>
       </c>
-      <c r="K11" s="1" t="n"/>
-      <c r="L11" s="1" t="n"/>
+      <c r="K11" s="33" t="n"/>
+      <c r="L11" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="120.75" r="12">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="33" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="33" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n"/>
+      <c r="A14" s="33" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Add EditAPI class in API and use it in main.py for updating dates
</commit_message>
<xml_diff>
--- a/4-08-2020 (2).xlsx
+++ b/4-08-2020 (2).xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="5" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Circle 6" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Circle 7 (2)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Circle 8 (3)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Circle 9 (4)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Circle 10 (5)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Circle 7" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Circle 8" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Circle 9" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Circle 10" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Circle 11" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
@@ -229,9 +229,6 @@
   </cellStyleXfs>
   <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -246,9 +243,6 @@
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -274,15 +268,6 @@
     <xf applyAlignment="1" borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -296,6 +281,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -724,11 +724,11 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="18.5703125"/>
@@ -741,8 +741,8 @@
     <col customWidth="1" max="11" min="11" style="29" width="18.140625"/>
     <col customWidth="1" max="12" min="12" style="29" width="14.140625"/>
     <col customWidth="1" max="13" min="13" style="29" width="10.85546875"/>
-    <col customWidth="1" max="14" min="14" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
+    <col customWidth="1" max="15" min="14" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="16" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -759,14 +759,14 @@
         </is>
       </c>
       <c r="C2" s="27" t="n"/>
-      <c r="J2" s="4" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Circle:6</t>
         </is>
       </c>
       <c r="K2" s="26" t="inlineStr">
         <is>
-          <t>09-09-2020</t>
+          <t>Date: 11-09-2020</t>
         </is>
       </c>
       <c r="L2" s="27" t="n"/>
@@ -863,18 +863,18 @@
       <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>Saidabad-24</t>
         </is>
       </c>
-      <c r="C5" s="13" t="inlineStr">
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t>Kaldev &amp;  
 9666977784</t>
         </is>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="11" t="n">
         <v>2.4</v>
       </c>
       <c r="E5" s="33" t="inlineStr">
@@ -905,21 +905,21 @@
       <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B6" s="7" t="inlineStr">
         <is>
           <t>Moosamrambagh-25</t>
         </is>
       </c>
-      <c r="C6" s="13" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>Jagadish &amp; 
 9505860994</t>
         </is>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D6" s="11" t="n">
         <v>2.3</v>
       </c>
-      <c r="E6" s="13" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>Sbi colony</t>
         </is>
@@ -946,7 +946,7 @@
       <c r="J6" s="33" t="n">
         <v>16.2</v>
       </c>
-      <c r="K6" s="9" t="inlineStr">
+      <c r="K6" s="7" t="inlineStr">
         <is>
           <t>Shalivana nagar,Moosarnbagh,Dilsuknagar,Gandhi nagar</t>
         </is>
@@ -957,18 +957,18 @@
       <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="7" t="inlineStr">
         <is>
           <t>Old Malakpet-26</t>
         </is>
       </c>
-      <c r="C7" s="13" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">Venugopal &amp; 
 9381278922 </t>
         </is>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="11" t="n">
         <v>2.5</v>
       </c>
       <c r="E7" s="33" t="inlineStr">
@@ -992,25 +992,25 @@
       </c>
       <c r="I7" s="33" t="n"/>
       <c r="J7" s="33" t="n"/>
-      <c r="K7" s="9" t="n"/>
+      <c r="K7" s="7" t="n"/>
       <c r="L7" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="8">
       <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>Azampura-28</t>
         </is>
       </c>
-      <c r="C8" s="13" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>Ganesh &amp; 
 9700484931</t>
         </is>
       </c>
-      <c r="D8" s="13" t="n">
+      <c r="D8" s="11" t="n">
         <v>2.6</v>
       </c>
       <c r="E8" s="33" t="inlineStr">
@@ -1041,18 +1041,18 @@
       <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>Dabeerpura-30</t>
         </is>
       </c>
-      <c r="C9" s="13" t="inlineStr">
+      <c r="C9" s="11" t="inlineStr">
         <is>
           <t>Ramesh &amp; 
 9247821824</t>
         </is>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="11" t="n">
         <v>2.4</v>
       </c>
       <c r="E9" s="33" t="inlineStr">
@@ -1074,7 +1074,7 @@
           <t>Shanker nagar new</t>
         </is>
       </c>
-      <c r="I9" s="11" t="inlineStr">
+      <c r="I9" s="9" t="inlineStr">
         <is>
           <t>B.Ravi
 9603268443</t>
@@ -1094,18 +1094,18 @@
       <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Akberbagh-27</t>
         </is>
       </c>
-      <c r="C10" s="13" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>Suresh &amp; 
 9985376352</t>
         </is>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="11" t="n">
         <v>2.2</v>
       </c>
       <c r="E10" s="33" t="inlineStr">
@@ -1136,18 +1136,18 @@
       <c r="A11" s="33" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Chowni-29</t>
         </is>
       </c>
-      <c r="C11" s="13" t="inlineStr">
+      <c r="C11" s="11" t="inlineStr">
         <is>
           <t>Jagadish &amp; 
 8886924293</t>
         </is>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="11" t="n">
         <v>2.7</v>
       </c>
       <c r="E11" s="33" t="inlineStr">
@@ -1230,7 +1230,7 @@
       <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="18.7109375"/>
@@ -1241,8 +1241,8 @@
     <col customWidth="1" max="10" min="9" style="29" width="14.140625"/>
     <col customWidth="1" max="11" min="11" style="29" width="18.28515625"/>
     <col customWidth="1" max="12" min="12" style="29" width="10.7109375"/>
-    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
+    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="C2" s="27" t="n"/>
-      <c r="J2" s="4" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Circle:7</t>
         </is>
@@ -1363,20 +1363,20 @@
       <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>Gowlipura-35</t>
         </is>
       </c>
-      <c r="C5" s="13" t="inlineStr">
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">Santosh &amp; 8555856896 </t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="E5" s="13" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>Kumarwadi Colony</t>
         </is>
@@ -1395,7 +1395,7 @@
           <t>Patel Nagar</t>
         </is>
       </c>
-      <c r="I5" s="10" t="inlineStr">
+      <c r="I5" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1405,7 +1405,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K5" s="8" t="inlineStr">
+      <c r="K5" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1416,20 +1416,20 @@
       <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B6" s="7" t="inlineStr">
         <is>
           <t>Rein Bazar-31</t>
         </is>
       </c>
-      <c r="C6" s="13" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>Narsimha &amp;  9985089596</t>
         </is>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="2" t="n">
         <v>2.6</v>
       </c>
-      <c r="E6" s="13" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>Surya Junghki dhawadi</t>
         </is>
@@ -1448,7 +1448,7 @@
           <t>Chandra Chota Nagar</t>
         </is>
       </c>
-      <c r="I6" s="10" t="inlineStr">
+      <c r="I6" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1458,7 +1458,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K6" s="8" t="inlineStr">
+      <c r="K6" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1469,21 +1469,21 @@
       <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="7" t="inlineStr">
         <is>
           <t>IS Sadan-38</t>
         </is>
       </c>
-      <c r="C7" s="13" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>Shanker
 9701554484</t>
         </is>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2" t="n">
         <v>2.2</v>
       </c>
-      <c r="E7" s="13" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>Laxmi Nagar</t>
         </is>
@@ -1497,12 +1497,12 @@
       <c r="G7" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H7" s="13" t="inlineStr">
+      <c r="H7" s="11" t="inlineStr">
         <is>
           <t>Sigareni Colony Huts</t>
         </is>
       </c>
-      <c r="I7" s="10" t="inlineStr">
+      <c r="I7" s="8" t="inlineStr">
         <is>
           <t>Abdul khaja hussain 9160969450</t>
         </is>
@@ -1521,20 +1521,20 @@
       <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>Kurmagdua-37</t>
         </is>
       </c>
-      <c r="C8" s="13" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>Babu &amp; 7981051446</t>
         </is>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="2" t="n">
         <v>2.3</v>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Medipur Madaanapet</t>
         </is>
@@ -1561,27 +1561,27 @@
       <c r="J8" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="K8" s="9" t="n"/>
+      <c r="K8" s="7" t="n"/>
       <c r="L8" s="34" t="n"/>
     </row>
     <row customHeight="1" ht="77.25" r="9">
       <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>Santoshnagar-39</t>
         </is>
       </c>
-      <c r="C9" s="13" t="inlineStr">
+      <c r="C9" s="11" t="inlineStr">
         <is>
           <t>Rajesh &amp; 8074007813</t>
         </is>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="2" t="n">
         <v>2.4</v>
       </c>
-      <c r="E9" s="13" t="inlineStr">
+      <c r="E9" s="11" t="inlineStr">
         <is>
           <t>Owasi Colony</t>
         </is>
@@ -1602,27 +1602,27 @@
       </c>
       <c r="I9" s="33" t="n"/>
       <c r="J9" s="33" t="n"/>
-      <c r="K9" s="9" t="n"/>
+      <c r="K9" s="7" t="n"/>
       <c r="L9" s="34" t="n"/>
     </row>
     <row customHeight="1" ht="106.5" r="10">
       <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Talabchachlam-34</t>
         </is>
       </c>
-      <c r="C10" s="13" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">Md Mujeeb &amp; 8919569079 </t>
         </is>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="E10" s="13" t="inlineStr">
+      <c r="E10" s="11" t="inlineStr">
         <is>
           <t>Bhavani Nagar</t>
         </is>
@@ -1636,12 +1636,12 @@
       <c r="G10" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H10" s="13" t="inlineStr">
+      <c r="H10" s="11" t="inlineStr">
         <is>
           <t>Bharani Nagar</t>
         </is>
       </c>
-      <c r="I10" s="10" t="inlineStr">
+      <c r="I10" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1651,7 +1651,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K10" s="8" t="inlineStr">
+      <c r="K10" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1717,7 +1717,7 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
@@ -1726,8 +1726,8 @@
     <col customWidth="1" max="9" min="5" style="29" width="14.140625"/>
     <col customWidth="1" max="10" min="10" style="29" width="13.5703125"/>
     <col customWidth="1" max="12" min="11" style="29" width="14.140625"/>
-    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
+    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -1744,7 +1744,7 @@
         </is>
       </c>
       <c r="C2" s="26" t="n"/>
-      <c r="J2" s="4" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Circle:8</t>
         </is>
@@ -1848,20 +1848,20 @@
       <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>Lalithabagh-36</t>
         </is>
       </c>
-      <c r="C5" s="13" t="inlineStr">
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t>Shiva Prasad &amp;  9618632623</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="2" t="n">
         <v>2.4</v>
       </c>
-      <c r="E5" s="13" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>Jyothi Bhag</t>
         </is>
@@ -1875,7 +1875,7 @@
       <c r="G5" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H5" s="13" t="inlineStr">
+      <c r="H5" s="11" t="inlineStr">
         <is>
           <t>Vinayak Nagar</t>
         </is>
@@ -1903,20 +1903,20 @@
       <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>Riyasthnagar-40</t>
         </is>
       </c>
-      <c r="C6" s="13" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>N Shanker &amp; 9502763663</t>
         </is>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="2" t="n">
         <v>2.3</v>
       </c>
-      <c r="E6" s="13" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>Jhamal Colony</t>
         </is>
@@ -1931,7 +1931,7 @@
       <c r="G6" s="33" t="n">
         <v>2.2</v>
       </c>
-      <c r="H6" s="13" t="inlineStr">
+      <c r="H6" s="11" t="inlineStr">
         <is>
           <t>Riyasath Nagar</t>
         </is>
@@ -1941,7 +1941,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J6" s="8" t="inlineStr">
+      <c r="J6" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1957,20 +1957,20 @@
       <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>Kanchanbagh-41</t>
         </is>
       </c>
-      <c r="C7" s="13" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">V Bharath &amp; 8801113420 </t>
         </is>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="13" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>A Block</t>
         </is>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="I7" s="33" t="n"/>
       <c r="J7" s="33" t="n"/>
-      <c r="K7" s="8" t="n"/>
+      <c r="K7" s="6" t="n"/>
       <c r="L7" s="33" t="inlineStr">
         <is>
           <t>-</t>
@@ -2002,17 +2002,17 @@
       <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>Barkas-42</t>
         </is>
       </c>
-      <c r="C8" s="13" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">Sathanarayana &amp; 7075705453 </t>
         </is>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="2" t="n">
         <v>2.3</v>
       </c>
       <c r="E8" s="33" t="inlineStr">
@@ -2034,7 +2034,7 @@
           <t>Ram Nagar</t>
         </is>
       </c>
-      <c r="I8" s="10" t="inlineStr">
+      <c r="I8" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2044,7 +2044,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K8" s="8" t="inlineStr">
+      <c r="K8" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2059,17 +2059,17 @@
       <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" s="1" t="inlineStr">
         <is>
           <t>Chandryangutta-43</t>
         </is>
       </c>
-      <c r="C9" s="13" t="inlineStr">
+      <c r="C9" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">Shaik Nayeem &amp; 9989431803 </t>
         </is>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="2" t="n">
         <v>2.7</v>
       </c>
       <c r="E9" s="29" t="inlineStr">
@@ -2100,7 +2100,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K9" s="8" t="inlineStr">
+      <c r="K9" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2115,17 +2115,17 @@
       <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="B10" s="1" t="inlineStr">
         <is>
           <t>Uppuguda-44</t>
         </is>
       </c>
-      <c r="C10" s="13" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>K Rakesh &amp; 9959636750</t>
         </is>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="2" t="n">
         <v>2.5</v>
       </c>
       <c r="E10" s="33" t="inlineStr">
@@ -2151,7 +2151,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J10" s="8" t="inlineStr">
+      <c r="J10" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2171,20 +2171,20 @@
       <c r="A11" s="33" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>Jangammet-45</t>
         </is>
       </c>
-      <c r="C11" s="13" t="inlineStr">
+      <c r="C11" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">C Manhohar &amp; 9059930220 </t>
         </is>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="2" t="n">
         <v>2.1</v>
       </c>
-      <c r="E11" s="13" t="inlineStr">
+      <c r="E11" s="11" t="inlineStr">
         <is>
           <t>Al Mustafa Colony</t>
         </is>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="I11" s="33" t="n"/>
       <c r="J11" s="33" t="n"/>
-      <c r="K11" s="8" t="n"/>
+      <c r="K11" s="6" t="n"/>
       <c r="L11" s="33" t="n"/>
     </row>
     <row customHeight="1" ht="50.25" r="12">
@@ -2256,15 +2256,15 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
     <col customWidth="1" max="3" min="3" style="29" width="15.7109375"/>
     <col customWidth="1" max="4" min="4" style="29" width="9.140625"/>
     <col customWidth="1" max="12" min="5" style="29" width="14.140625"/>
-    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
+    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -2281,7 +2281,7 @@
         </is>
       </c>
       <c r="C2" s="26" t="n"/>
-      <c r="J2" s="4" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Circle:9</t>
         </is>
@@ -2385,20 +2385,20 @@
       <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Pathergatti-32</t>
         </is>
       </c>
-      <c r="C5" s="13" t="inlineStr">
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t>Shiva &amp;  9502535493</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="2" t="n">
         <v>2.2</v>
       </c>
-      <c r="E5" s="13" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>Unani Hospital</t>
         </is>
@@ -2442,20 +2442,20 @@
       <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>Shalibanda-48</t>
         </is>
       </c>
-      <c r="C6" s="13" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>Ali baba &amp; 8328654875</t>
         </is>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="2" t="n">
         <v>2.4</v>
       </c>
-      <c r="E6" s="13" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>Khaji Pura</t>
         </is>
@@ -2499,20 +2499,20 @@
       <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Puranapul-52</t>
         </is>
       </c>
-      <c r="C7" s="13" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>MD Majid &amp; 7780173117</t>
         </is>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="13" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>Aligulsham</t>
         </is>
@@ -2556,20 +2556,20 @@
       <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
         <is>
           <t>Moghalpura-33</t>
         </is>
       </c>
-      <c r="C8" s="13" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">Kirankuamar &amp; 9398465271 </t>
         </is>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="2" t="n">
         <v>2.6</v>
       </c>
-      <c r="E8" s="13" t="inlineStr">
+      <c r="E8" s="11" t="inlineStr">
         <is>
           <t>Moghalpura Water Tank</t>
         </is>
@@ -2583,7 +2583,7 @@
       <c r="G8" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H8" s="13" t="inlineStr">
+      <c r="H8" s="11" t="inlineStr">
         <is>
           <t>Billa Colony</t>
         </is>
@@ -2604,25 +2604,25 @@
       <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>Ghansibazar-49</t>
         </is>
       </c>
-      <c r="C9" s="13" t="inlineStr">
+      <c r="C9" s="11" t="inlineStr">
         <is>
           <t>Bikshapathi &amp;  6302782341</t>
         </is>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="2" t="n">
         <v>2.1</v>
       </c>
-      <c r="E9" s="13" t="inlineStr">
+      <c r="E9" s="11" t="inlineStr">
         <is>
           <t>Husain Alam</t>
         </is>
       </c>
-      <c r="F9" s="12" t="inlineStr">
+      <c r="F9" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">Arjun
 8801838776
@@ -2632,7 +2632,7 @@
       <c r="G9" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H9" s="13" t="inlineStr">
+      <c r="H9" s="11" t="inlineStr">
         <is>
           <t>Musa Bowli</t>
         </is>
@@ -2705,7 +2705,7 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
@@ -2714,8 +2714,8 @@
     <col customWidth="1" max="10" min="5" style="29" width="14.140625"/>
     <col customWidth="1" max="11" min="11" style="29" width="19"/>
     <col customWidth="1" max="12" min="12" style="29" width="14.140625"/>
-    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
+    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -2732,7 +2732,7 @@
         </is>
       </c>
       <c r="C2" s="27" t="n"/>
-      <c r="J2" s="4" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Circle:10</t>
         </is>
@@ -2745,42 +2745,42 @@
       <c r="L2" s="27" t="n"/>
     </row>
     <row customHeight="1" ht="30.75" r="3">
-      <c r="A3" s="19" t="inlineStr">
+      <c r="A3" s="14" t="inlineStr">
         <is>
           <t>SL No</t>
         </is>
       </c>
-      <c r="B3" s="19" t="inlineStr">
+      <c r="B3" s="14" t="inlineStr">
         <is>
           <t>Division Name</t>
         </is>
       </c>
-      <c r="C3" s="20" t="inlineStr">
+      <c r="C3" s="15" t="inlineStr">
         <is>
           <t>PFM-1</t>
         </is>
       </c>
-      <c r="D3" s="21" t="n"/>
-      <c r="E3" s="22" t="n"/>
-      <c r="F3" s="20" t="inlineStr">
+      <c r="D3" s="16" t="n"/>
+      <c r="E3" s="17" t="n"/>
+      <c r="F3" s="15" t="inlineStr">
         <is>
           <t>PFM-2</t>
         </is>
       </c>
-      <c r="G3" s="21" t="n"/>
-      <c r="H3" s="22" t="n"/>
-      <c r="I3" s="20" t="inlineStr">
+      <c r="G3" s="16" t="n"/>
+      <c r="H3" s="17" t="n"/>
+      <c r="I3" s="15" t="inlineStr">
         <is>
           <t>VMF</t>
         </is>
       </c>
-      <c r="J3" s="21" t="n"/>
-      <c r="K3" s="22" t="n"/>
+      <c r="J3" s="16" t="n"/>
+      <c r="K3" s="17" t="n"/>
       <c r="L3" s="30" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="4">
-      <c r="A4" s="23" t="n"/>
-      <c r="B4" s="23" t="n"/>
+      <c r="A4" s="18" t="n"/>
+      <c r="B4" s="18" t="n"/>
       <c r="C4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
@@ -2836,20 +2836,20 @@
       <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Dhood Bowli-53</t>
         </is>
       </c>
-      <c r="C5" s="13" t="inlineStr">
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t>Md Riyaz &amp; 9398135298</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="2" t="n">
         <v>2.6</v>
       </c>
-      <c r="E5" s="13" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>Fathedharwasa</t>
         </is>
@@ -2891,20 +2891,20 @@
       <c r="A6" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>Ramnaspura-55</t>
         </is>
       </c>
-      <c r="C6" s="13" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">MD Waseem &amp; 8801984231 </t>
         </is>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="2" t="n">
         <v>2.2</v>
       </c>
-      <c r="E6" s="13" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>Khaja Pahadi</t>
         </is>
@@ -2932,20 +2932,20 @@
       <c r="A7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Jahanuma-54</t>
         </is>
       </c>
-      <c r="C7" s="13" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>Jagdishwaer &amp; 9533744179</t>
         </is>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="E7" s="13" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>Pulbhag</t>
         </is>
@@ -2964,7 +2964,7 @@
           <t>Jahanuma</t>
         </is>
       </c>
-      <c r="I7" s="14" t="inlineStr">
+      <c r="I7" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2974,7 +2974,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K7" s="15" t="inlineStr">
+      <c r="K7" s="13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2989,17 +2989,17 @@
       <c r="A8" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
         <is>
           <t>Kishanbagh-56</t>
         </is>
       </c>
-      <c r="C8" s="13" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>Mahender &amp; 9700705283</t>
         </is>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="2" t="n">
         <v>2.2</v>
       </c>
       <c r="E8" s="33" t="inlineStr">
@@ -3015,7 +3015,7 @@
       <c r="G8" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H8" s="13" t="inlineStr">
+      <c r="H8" s="11" t="inlineStr">
         <is>
           <t>Kishanbhagh</t>
         </is>
@@ -3027,20 +3027,20 @@
       <c r="A9" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>Nawabshab Kunta-47</t>
         </is>
       </c>
-      <c r="C9" s="13" t="inlineStr">
+      <c r="C9" s="11" t="inlineStr">
         <is>
           <t>Arjun &amp; 8501890109</t>
         </is>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="2" t="n">
         <v>2.3</v>
       </c>
-      <c r="E9" s="13" t="inlineStr">
+      <c r="E9" s="11" t="inlineStr">
         <is>
           <t>Janumalalsar</t>
         </is>
@@ -3053,7 +3053,7 @@
       <c r="G9" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H9" s="13" t="inlineStr">
+      <c r="H9" s="11" t="inlineStr">
         <is>
           <t>Sanjay Gandhi nagar</t>
         </is>
@@ -3079,20 +3079,20 @@
       <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>Falaknuma-46</t>
         </is>
       </c>
-      <c r="C10" s="13" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>S Raju &amp;  9440993466</t>
         </is>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="11" t="n">
         <v>2.2</v>
       </c>
-      <c r="E10" s="13" t="inlineStr">
+      <c r="E10" s="11" t="inlineStr">
         <is>
           <t>Aljabal Colony</t>
         </is>
@@ -3173,11 +3173,11 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
@@ -3188,8 +3188,8 @@
     <col customWidth="1" max="7" min="7" style="29" width="11.28515625"/>
     <col customWidth="1" max="8" min="8" style="29" width="16.5703125"/>
     <col customWidth="1" max="12" min="9" style="29" width="14.140625"/>
-    <col customWidth="1" max="13" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="14" style="29" width="9.140625"/>
+    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -3206,7 +3206,7 @@
         </is>
       </c>
       <c r="C2" s="26" t="n"/>
-      <c r="J2" s="4" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Circle:11</t>
         </is>
@@ -3219,36 +3219,36 @@
       <c r="L2" s="26" t="n"/>
     </row>
     <row r="3">
-      <c r="B3" s="19" t="inlineStr">
+      <c r="B3" s="14" t="inlineStr">
         <is>
           <t>Division Name</t>
         </is>
       </c>
-      <c r="C3" s="20" t="inlineStr">
+      <c r="C3" s="15" t="inlineStr">
         <is>
           <t>PFM-1</t>
         </is>
       </c>
-      <c r="D3" s="21" t="n"/>
-      <c r="E3" s="22" t="n"/>
-      <c r="F3" s="20" t="inlineStr">
+      <c r="D3" s="16" t="n"/>
+      <c r="E3" s="17" t="n"/>
+      <c r="F3" s="15" t="inlineStr">
         <is>
           <t>PFM-2</t>
         </is>
       </c>
-      <c r="G3" s="21" t="n"/>
-      <c r="H3" s="22" t="n"/>
-      <c r="I3" s="20" t="inlineStr">
+      <c r="G3" s="16" t="n"/>
+      <c r="H3" s="17" t="n"/>
+      <c r="I3" s="15" t="inlineStr">
         <is>
           <t>VMF</t>
         </is>
       </c>
-      <c r="J3" s="21" t="n"/>
-      <c r="K3" s="22" t="n"/>
+      <c r="J3" s="16" t="n"/>
+      <c r="K3" s="17" t="n"/>
       <c r="L3" s="30" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="4">
-      <c r="B4" s="23" t="n"/>
+      <c r="B4" s="18" t="n"/>
       <c r="C4" s="30" t="inlineStr">
         <is>
           <t>TL Name &amp; Mobile</t>
@@ -3299,20 +3299,20 @@
       </c>
     </row>
     <row customHeight="1" ht="34.5" r="5">
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Suleman nagar-57</t>
         </is>
       </c>
-      <c r="C5" s="13" t="inlineStr">
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t>K Suresh Kumar &amp; 9848486473</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="E5" s="13" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>Koi Muhamad</t>
         </is>
@@ -3346,20 +3346,20 @@
           <t>SL No</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>Shastripuram-58</t>
         </is>
       </c>
-      <c r="C6" s="13" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>M Vishnuvardhan &amp; 9700286845</t>
         </is>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="2" t="n">
         <v>2.4</v>
       </c>
-      <c r="E6" s="13" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>Ashan Nagar</t>
         </is>
@@ -3373,7 +3373,7 @@
       <c r="G6" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H6" s="13" t="inlineStr">
+      <c r="H6" s="11" t="inlineStr">
         <is>
           <t>Owasi Hills</t>
         </is>
@@ -3387,7 +3387,7 @@
       <c r="J6" s="33" t="n">
         <v>17</v>
       </c>
-      <c r="K6" s="8" t="inlineStr">
+      <c r="K6" s="6" t="inlineStr">
         <is>
           <t>BK puram, Vattapalli, Shasthri Puram</t>
         </is>
@@ -3400,20 +3400,20 @@
     </row>
     <row customHeight="1" ht="36" r="7">
       <c r="A7" s="31" t="n"/>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Mailerdevpally-59</t>
         </is>
       </c>
-      <c r="C7" s="13" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>K Vinod Kumar &amp; 8309606521</t>
         </is>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2" t="n">
         <v>2.2</v>
       </c>
-      <c r="E7" s="13" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>Aaranghar</t>
         </is>
@@ -3427,7 +3427,7 @@
       <c r="G7" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="H7" s="13" t="inlineStr">
+      <c r="H7" s="11" t="inlineStr">
         <is>
           <t>NTR nagar</t>
         </is>
@@ -3445,20 +3445,20 @@
       <c r="A8" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
         <is>
           <t>Rajendranagar-60</t>
         </is>
       </c>
-      <c r="C8" s="13" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>Y Gopal &amp; 9346854806</t>
         </is>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="2" t="n">
         <v>2.6</v>
       </c>
-      <c r="E8" s="13" t="inlineStr">
+      <c r="E8" s="11" t="inlineStr">
         <is>
           <t>Yadav Reddy Nagar</t>
         </is>
@@ -3472,7 +3472,7 @@
       <c r="G8" s="33" t="n">
         <v>2.4</v>
       </c>
-      <c r="H8" s="13" t="inlineStr">
+      <c r="H8" s="11" t="inlineStr">
         <is>
           <t>Uppar Palli</t>
         </is>
@@ -3490,20 +3490,20 @@
       <c r="A9" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>Attapur-61</t>
         </is>
       </c>
-      <c r="C9" s="13" t="inlineStr">
+      <c r="C9" s="11" t="inlineStr">
         <is>
           <t>Hyder guda</t>
         </is>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="2" t="n">
         <v>2.4</v>
       </c>
-      <c r="E9" s="13" t="inlineStr">
+      <c r="E9" s="11" t="inlineStr">
         <is>
           <t>Khaj Nagar</t>
         </is>
@@ -3517,12 +3517,12 @@
       <c r="G9" s="33" t="n">
         <v>2.6</v>
       </c>
-      <c r="H9" s="13" t="inlineStr">
+      <c r="H9" s="11" t="inlineStr">
         <is>
           <t>Bharat Nagar</t>
         </is>
       </c>
-      <c r="I9" s="11" t="inlineStr">
+      <c r="I9" s="9" t="inlineStr">
         <is>
           <t>Ravi
 6302097148</t>
@@ -3531,7 +3531,7 @@
       <c r="J9" s="33" t="n">
         <v>18.5</v>
       </c>
-      <c r="K9" s="8" t="inlineStr">
+      <c r="K9" s="6" t="inlineStr">
         <is>
           <t>Attapur Daltha Basthi, Bhagi Nagar, Indra Nagar, Tejeshwini colony</t>
         </is>
@@ -3546,20 +3546,20 @@
       <c r="A10" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>Complaint Machine</t>
         </is>
       </c>
-      <c r="C10" s="13" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>Shyamsunder &amp; 8125247675</t>
         </is>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="E10" s="13" t="inlineStr">
+      <c r="E10" s="11" t="inlineStr">
         <is>
           <t>Rhagavendra Nagar</t>
         </is>
@@ -3575,7 +3575,7 @@
         </is>
       </c>
       <c r="H10" s="33" t="n"/>
-      <c r="I10" s="10" t="inlineStr">
+      <c r="I10" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3585,7 +3585,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K10" s="8" t="inlineStr">
+      <c r="K10" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
Complete TODO, update 'update_date' function to avoid redundantly updating date in new API
</commit_message>
<xml_diff>
--- a/4-08-2020 (2).xlsx
+++ b/4-08-2020 (2).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="5" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Circle 6" sheetId="1" state="visible" r:id="rId1"/>
@@ -724,11 +724,11 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="18.5703125"/>
@@ -741,8 +741,8 @@
     <col customWidth="1" max="11" min="11" style="29" width="18.140625"/>
     <col customWidth="1" max="12" min="12" style="29" width="14.140625"/>
     <col customWidth="1" max="13" min="13" style="29" width="10.85546875"/>
-    <col customWidth="1" max="15" min="14" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="16" style="29" width="9.140625"/>
+    <col customWidth="1" max="16" min="14" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="17" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -1230,7 +1230,7 @@
       <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="18.7109375"/>
@@ -1241,8 +1241,8 @@
     <col customWidth="1" max="10" min="9" style="29" width="14.140625"/>
     <col customWidth="1" max="11" min="11" style="29" width="18.28515625"/>
     <col customWidth="1" max="12" min="12" style="29" width="10.7109375"/>
-    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
+    <col customWidth="1" max="15" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="16" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -1717,7 +1717,7 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
@@ -1726,8 +1726,8 @@
     <col customWidth="1" max="9" min="5" style="29" width="14.140625"/>
     <col customWidth="1" max="10" min="10" style="29" width="13.5703125"/>
     <col customWidth="1" max="12" min="11" style="29" width="14.140625"/>
-    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
+    <col customWidth="1" max="15" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="16" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -2256,15 +2256,15 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
     <col customWidth="1" max="3" min="3" style="29" width="15.7109375"/>
     <col customWidth="1" max="4" min="4" style="29" width="9.140625"/>
     <col customWidth="1" max="12" min="5" style="29" width="14.140625"/>
-    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
+    <col customWidth="1" max="15" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="16" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -2705,7 +2705,7 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
@@ -2714,8 +2714,8 @@
     <col customWidth="1" max="10" min="5" style="29" width="14.140625"/>
     <col customWidth="1" max="11" min="11" style="29" width="19"/>
     <col customWidth="1" max="12" min="12" style="29" width="14.140625"/>
-    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
+    <col customWidth="1" max="15" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="16" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -3173,11 +3173,11 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="29" width="4.42578125"/>
     <col customWidth="1" max="2" min="2" style="29" width="17.7109375"/>
@@ -3188,8 +3188,8 @@
     <col customWidth="1" max="7" min="7" style="29" width="11.28515625"/>
     <col customWidth="1" max="8" min="8" style="29" width="16.5703125"/>
     <col customWidth="1" max="12" min="9" style="29" width="14.140625"/>
-    <col customWidth="1" max="14" min="13" style="29" width="9.140625"/>
-    <col customWidth="1" max="16384" min="15" style="29" width="9.140625"/>
+    <col customWidth="1" max="15" min="13" style="29" width="9.140625"/>
+    <col customWidth="1" max="16384" min="16" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">

</xml_diff>

<commit_message>
Convert entire codebase to kv
</commit_message>
<xml_diff>
--- a/4-08-2020 (2).xlsx
+++ b/4-08-2020 (2).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\Python WorkSpace\Projects\report-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A13819B-57A6-4511-8626-8622ED58D159}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141BB9AE-B4D1-4576-8C48-E2A1508C8415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
     <t>Circle:6</t>
   </si>
   <si>
-    <t>Date: 11-09-2020</t>
+    <t>Date: 17-09-2020</t>
   </si>
   <si>
     <t>SL No</t>
@@ -175,9 +175,6 @@
 8074162170</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Rein Bazar-31</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   <si>
     <t>Masood 
 939841342</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>Riyasthnagar-40</t>
@@ -1105,8 +1105,8 @@
     <col min="11" max="11" width="18.140625" style="21" customWidth="1"/>
     <col min="12" max="12" width="14.140625" style="21" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="21" customWidth="1"/>
-    <col min="14" max="17" width="9.140625" style="21" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="21"/>
+    <col min="14" max="18" width="9.140625" style="21" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1206,12 +1206,16 @@
       <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
       <c r="E5" s="23"/>
       <c r="F5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="23"/>
+      <c r="G5" s="23">
+        <v>0</v>
+      </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
@@ -1228,12 +1232,16 @@
       <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
       <c r="E6" s="11"/>
       <c r="F6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="23"/>
+      <c r="G6" s="23">
+        <v>0</v>
+      </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
@@ -1250,12 +1258,16 @@
       <c r="C7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
       <c r="E7" s="23"/>
       <c r="F7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="23">
+        <v>0</v>
+      </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
@@ -1272,12 +1284,16 @@
       <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
       <c r="E8" s="23"/>
       <c r="F8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="23"/>
+      <c r="G8" s="23">
+        <v>0</v>
+      </c>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
@@ -1294,12 +1310,16 @@
       <c r="C9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
       <c r="E9" s="23"/>
       <c r="F9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="23"/>
+      <c r="G9" s="23">
+        <v>0</v>
+      </c>
       <c r="H9" s="23"/>
       <c r="I9" s="9"/>
       <c r="J9" s="23"/>
@@ -1316,12 +1336,16 @@
       <c r="C10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
       <c r="E10" s="23"/>
       <c r="F10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="23"/>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
@@ -1338,12 +1362,16 @@
       <c r="C11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
       <c r="E11" s="23"/>
       <c r="F11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="23">
+        <v>0</v>
+      </c>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
@@ -1411,8 +1439,8 @@
     <col min="9" max="10" width="14.140625" style="21" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" style="21" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" style="21" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="21" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="21"/>
+    <col min="13" max="17" width="9.140625" style="21" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,15 +1557,15 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="11"/>
       <c r="F6" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -1551,15 +1579,15 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="11"/>
       <c r="F7" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="11"/>
@@ -1573,15 +1601,15 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
@@ -1595,15 +1623,15 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="11"/>
       <c r="F9" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -1617,15 +1645,15 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="11"/>
       <c r="F10" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="11"/>
@@ -1696,8 +1724,8 @@
     <col min="5" max="9" width="14.140625" style="21" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" style="21" customWidth="1"/>
     <col min="11" max="12" width="14.140625" style="21" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="21" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="21"/>
+    <col min="13" max="17" width="9.140625" style="21" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1722,7 +1750,7 @@
       </c>
       <c r="C2" s="20"/>
       <c r="J2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>37</v>
@@ -1792,15 +1820,15 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="11"/>
       <c r="F5" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="11"/>
@@ -1808,7 +1836,7 @@
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
       <c r="L5" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1829,13 +1857,13 @@
       <c r="G6" s="23"/>
       <c r="H6" s="11"/>
       <c r="I6" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="L6" s="23"/>
     </row>
@@ -1860,7 +1888,7 @@
       <c r="J7" s="23"/>
       <c r="K7" s="6"/>
       <c r="L7" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1881,16 +1909,16 @@
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="8" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1909,16 +1937,16 @@
       </c>
       <c r="G9" s="23"/>
       <c r="I9" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1939,16 +1967,16 @@
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
@@ -2010,10 +2038,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="L11" sqref="A11:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,8 +2051,8 @@
     <col min="3" max="3" width="15.7109375" style="21" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="21" customWidth="1"/>
     <col min="5" max="12" width="14.140625" style="21" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="21" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="21"/>
+    <col min="13" max="17" width="9.140625" style="21" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2052,7 +2080,7 @@
         <v>79</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="L2" s="20"/>
     </row>
@@ -2124,18 +2152,24 @@
       <c r="C5" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
       <c r="E5" s="11"/>
       <c r="F5" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="23"/>
+      <c r="G5" s="23">
+        <v>0</v>
+      </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
+      <c r="J5" s="23">
+        <v>0</v>
+      </c>
       <c r="K5" s="23"/>
       <c r="L5" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2148,18 +2182,24 @@
       <c r="C6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
       <c r="E6" s="11"/>
       <c r="F6" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="23"/>
+      <c r="G6" s="23">
+        <v>0</v>
+      </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
+      <c r="J6" s="23">
+        <v>0</v>
+      </c>
       <c r="K6" s="23"/>
       <c r="L6" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2172,18 +2212,24 @@
       <c r="C7" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
       <c r="E7" s="11"/>
       <c r="F7" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="23">
+        <v>0</v>
+      </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
+      <c r="J7" s="23">
+        <v>0</v>
+      </c>
       <c r="K7" s="23"/>
       <c r="L7" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2196,14 +2242,21 @@
       <c r="C8" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
       <c r="E8" s="11"/>
       <c r="F8" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="23"/>
+      <c r="G8" s="23">
+        <v>0</v>
+      </c>
       <c r="H8" s="11"/>
-      <c r="J8" s="23"/>
+      <c r="I8"/>
+      <c r="J8" s="23">
+        <v>0</v>
+      </c>
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
     </row>
@@ -2217,18 +2270,24 @@
       <c r="C9" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
       <c r="E9" s="11"/>
       <c r="F9" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G9" s="23"/>
+      <c r="G9" s="23">
+        <v>0</v>
+      </c>
       <c r="H9" s="11"/>
       <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
+      <c r="J9" s="23">
+        <v>0</v>
+      </c>
       <c r="K9" s="23"/>
       <c r="L9" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2238,20 +2297,29 @@
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="19">
-        <f>SUM(D5:D9)</f>
         <v>0</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="22">
-        <f>SUM(G5:G9)</f>
         <v>0</v>
       </c>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
-      <c r="J10" s="22"/>
+      <c r="J10" s="22">
+        <v>0</v>
+      </c>
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2280,8 +2348,8 @@
     <col min="5" max="10" width="14.140625" style="21" customWidth="1"/>
     <col min="11" max="11" width="19" style="21" customWidth="1"/>
     <col min="12" max="12" width="14.140625" style="21" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="21" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="21"/>
+    <col min="13" max="17" width="9.140625" style="21" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2392,7 +2460,7 @@
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
       <c r="L5" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2435,14 +2503,14 @@
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="12" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="13" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2483,11 +2551,11 @@
       <c r="G9" s="23"/>
       <c r="H9" s="11"/>
       <c r="I9" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="L9" s="23"/>
     </row>
@@ -2509,11 +2577,11 @@
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J10" s="23"/>
       <c r="K10" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="L10" s="23"/>
     </row>
@@ -2553,10 +2621,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2570,8 +2638,8 @@
     <col min="7" max="7" width="11.28515625" style="21" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" style="21" customWidth="1"/>
     <col min="9" max="12" width="14.140625" style="21" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="21" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="21"/>
+    <col min="13" max="17" width="9.140625" style="21" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2624,7 +2692,7 @@
       <c r="K3" s="17"/>
       <c r="L3" s="22"/>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18"/>
       <c r="C4" s="22" t="s">
         <v>9</v>
@@ -2675,7 +2743,7 @@
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
       <c r="L5" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2699,7 +2767,7 @@
       <c r="J6" s="23"/>
       <c r="K6" s="6"/>
       <c r="L6" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2721,7 +2789,7 @@
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
       <c r="L7" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2745,7 +2813,7 @@
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
       <c r="L8" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -2769,7 +2837,7 @@
       <c r="J9" s="23"/>
       <c r="K9" s="6"/>
       <c r="L9" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2785,7 +2853,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="11"/>
       <c r="F10" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -2793,7 +2861,7 @@
       <c r="J10" s="23"/>
       <c r="K10" s="6"/>
       <c r="L10" s="23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2823,19 +2891,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
     </row>
-    <row r="12" spans="1:12" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-    </row>
+    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A6:A7"/>

</xml_diff>